<commit_message>
adding support to description on the MGMT interface
</commit_message>
<xml_diff>
--- a/spreadsheets/ipn.xlsx
+++ b/spreadsheets/ipn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassio/PycharmProjects/ipn_isn_automation/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calange/PycharmProjects/ipn_isn_automation/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A035DB-06B0-5645-898E-8A91FEC6DAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6467F20-2907-A34C-9B3E-8C1FD571C5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14060" yWindow="-28800" windowWidth="68800" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15700" yWindow="-28800" windowWidth="68800" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="6" r:id="rId1"/>
@@ -68,19 +68,10 @@
   <commentList>
     <comment ref="G2" authorId="0" shapeId="0" xr:uid="{74DB15BE-2946-4C4C-8FDC-9E0C548F5A2A}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Ibf8x$FHLU$L6mAz</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -88,14 +79,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -110,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="450">
   <si>
     <t>HOSTNAME</t>
   </si>
@@ -1457,6 +1448,9 @@
   </si>
   <si>
     <t>SERIAL_NUMBER</t>
+  </si>
+  <si>
+    <t>MGMT_DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -1673,7 +1667,25 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{7E5BFF21-FF29-42C5-8362-8040CB29CF6C}"/>
   </cellStyles>
-  <dxfs count="100">
+  <dxfs count="101">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -3724,17 +3736,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{509596C7-D353-D14A-BD3B-3A0CCF6D18AE}" name="devices" displayName="devices" ref="A1:P2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:P2" xr:uid="{6F3A0D7A-D722-E743-99ED-9A12FCB8C763}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{381CC9EE-E379-3949-8A0B-9662994EC61F}" name="HOSTNAME" dataDxfId="99"/>
-    <tableColumn id="16" xr3:uid="{D41A0F4C-32E3-DC40-BE24-4D9B419C9A57}" name="SERIAL_NUMBER" dataDxfId="98"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{509596C7-D353-D14A-BD3B-3A0CCF6D18AE}" name="devices" displayName="devices" ref="A1:Q2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:Q2" xr:uid="{6F3A0D7A-D722-E743-99ED-9A12FCB8C763}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{381CC9EE-E379-3949-8A0B-9662994EC61F}" name="HOSTNAME" dataDxfId="100"/>
+    <tableColumn id="16" xr3:uid="{D41A0F4C-32E3-DC40-BE24-4D9B419C9A57}" name="SERIAL_NUMBER" dataDxfId="99"/>
     <tableColumn id="2" xr3:uid="{DF76891E-9FEE-364E-950B-D2AF1487DE91}" name="DEVICE_OS"/>
     <tableColumn id="7" xr3:uid="{599A17A7-36B0-5E42-BB84-35BAA37040F9}" name="DEVICE_TYPE"/>
     <tableColumn id="3" xr3:uid="{CB026E15-2101-8E49-B5EA-A19D5EA278E1}" name="MGMT_INT"/>
-    <tableColumn id="4" xr3:uid="{10B5AEE1-2F46-8140-80E7-23A7CF06F12B}" name="MGMT_VRF" dataDxfId="97"/>
-    <tableColumn id="5" xr3:uid="{8E625E2F-DFC3-1E47-9623-DFDC9AA7CC26}" name="MGMT_IP" dataDxfId="96"/>
-    <tableColumn id="6" xr3:uid="{381A8401-24A4-7F45-8DCA-CA9B15CACEA9}" name="MGMT_GW" dataDxfId="95"/>
+    <tableColumn id="4" xr3:uid="{10B5AEE1-2F46-8140-80E7-23A7CF06F12B}" name="MGMT_VRF" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{8E625E2F-DFC3-1E47-9623-DFDC9AA7CC26}" name="MGMT_IP" dataDxfId="97"/>
+    <tableColumn id="6" xr3:uid="{381A8401-24A4-7F45-8DCA-CA9B15CACEA9}" name="MGMT_GW" dataDxfId="96"/>
+    <tableColumn id="17" xr3:uid="{107D9780-9B12-CC4B-8637-1943D81E2D2E}" name="MGMT_DESCRIPTION" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{FD91D019-1042-1A4B-9C02-3E16ECD3C6B8}" name="USERNAME"/>
     <tableColumn id="9" xr3:uid="{9016DBD0-0BD9-B44A-87D7-39611823CBC1}" name="PASSWORD"/>
     <tableColumn id="10" xr3:uid="{7BDC3620-DB6A-ED45-B7EF-A52B60E5A63A}" name="ENABLE"/>
@@ -3749,33 +3762,33 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{66160081-DEC2-404A-B86C-A5A1FE0E2385}" name="prefix_list" displayName="prefix_list" ref="A1:K2" insertRow="1" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{66160081-DEC2-404A-B86C-A5A1FE0E2385}" name="prefix_list" displayName="prefix_list" ref="A1:K2" insertRow="1" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
   <autoFilter ref="A1:K2" xr:uid="{D55CF0F7-6E4A-BF4C-918F-5A724EA4861F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F2D78B99-533C-B649-93FC-1E9C4AF83F80}" name="HOSTNAME" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{17B5652C-C4F7-004A-8AF1-BABF5656C432}" name="DEVICE_OS" dataDxfId="57">
+    <tableColumn id="1" xr3:uid="{F2D78B99-533C-B649-93FC-1E9C4AF83F80}" name="HOSTNAME" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{17B5652C-C4F7-004A-8AF1-BABF5656C432}" name="DEVICE_OS" dataDxfId="58">
       <calculatedColumnFormula>IF(ISBLANK(prefix_list[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(prefix_list[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F9A61C22-2FDA-A642-AA1F-8E9A458C6039}" name="NAME" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{1C364EF9-1AFD-2D4B-B61D-1591B410DD90}" name="DESCRIPTION" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{35AA2362-D924-F44C-B2F2-40764BA64F59}" name="ADDRESS_FAMILY" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{88DA9E15-E49F-1849-9616-0F4813B909F5}" name="SEQUENCE" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{9296DC93-138E-114B-81F3-49030054A86C}" name="ACTION" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{9FF719D3-00E1-634D-8391-AD1803B05B20}" name="PREFIX" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{D1D60C28-AF41-5F4F-ABB6-02186395F57B}" name="GE" dataDxfId="50"/>
-    <tableColumn id="10" xr3:uid="{1E602C71-DB91-C04B-912A-1D1DDE852D43}" name="LE" dataDxfId="49"/>
-    <tableColumn id="11" xr3:uid="{5BCFBE35-DC23-4440-884F-5291013B2AD8}" name="STATUS" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{F9A61C22-2FDA-A642-AA1F-8E9A458C6039}" name="NAME" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{1C364EF9-1AFD-2D4B-B61D-1591B410DD90}" name="DESCRIPTION" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{35AA2362-D924-F44C-B2F2-40764BA64F59}" name="ADDRESS_FAMILY" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{88DA9E15-E49F-1849-9616-0F4813B909F5}" name="SEQUENCE" dataDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{9296DC93-138E-114B-81F3-49030054A86C}" name="ACTION" dataDxfId="53"/>
+    <tableColumn id="8" xr3:uid="{9FF719D3-00E1-634D-8391-AD1803B05B20}" name="PREFIX" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{D1D60C28-AF41-5F4F-ABB6-02186395F57B}" name="GE" dataDxfId="51"/>
+    <tableColumn id="10" xr3:uid="{1E602C71-DB91-C04B-912A-1D1DDE852D43}" name="LE" dataDxfId="50"/>
+    <tableColumn id="11" xr3:uid="{5BCFBE35-DC23-4440-884F-5291013B2AD8}" name="STATUS" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6E452009-DEEF-5C4C-85C0-8D759B63A698}" name="route_map" displayName="route_map" ref="A1:M2" insertRow="1" totalsRowShown="0" tableBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6E452009-DEEF-5C4C-85C0-8D759B63A698}" name="route_map" displayName="route_map" ref="A1:M2" insertRow="1" totalsRowShown="0" tableBorderDxfId="48">
   <autoFilter ref="A1:M2" xr:uid="{97EDB19E-68E0-B14D-837F-27C451B5CB8C}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{3BDEDE97-72E9-C84A-9F44-E18054506FE4}" name="HOSTNAME" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{7506AE33-5FAA-044A-8B2B-E417F16E93C8}" name="DEVICE_OS" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{3BDEDE97-72E9-C84A-9F44-E18054506FE4}" name="HOSTNAME" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{7506AE33-5FAA-044A-8B2B-E417F16E93C8}" name="DEVICE_OS" dataDxfId="46">
       <calculatedColumnFormula>IF(ISBLANK(route_map[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(route_map[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{1F665B2D-B35E-FC4D-9C4C-B9595DC2D3F7}" name="NAME"/>
@@ -3784,77 +3797,77 @@
     <tableColumn id="5" xr3:uid="{91A7A709-9BA1-4743-BFBA-C980FCA55C61}" name="ACTION"/>
     <tableColumn id="6" xr3:uid="{37FEFFEE-58D5-BF47-A6AC-D4DB9D9CD4EC}" name="PREFIX_LIST"/>
     <tableColumn id="7" xr3:uid="{089E8480-CD75-2F45-93E1-67BA2B42FF21}" name="AS_PATH_ACCESS_LIST"/>
-    <tableColumn id="8" xr3:uid="{F9459908-C24B-9144-8097-1F11F1CB8FFA}" name="AS_PATH_ACCESS_LIST_NUMBER" dataDxfId="44">
+    <tableColumn id="8" xr3:uid="{F9459908-C24B-9144-8097-1F11F1CB8FFA}" name="AS_PATH_ACCESS_LIST_NUMBER" dataDxfId="45">
       <calculatedColumnFormula>IF(ISBLANK(route_map[[#This Row],[AS_PATH_ACCESS_LIST]]),"",_xlfn.XLOOKUP(route_map[[#This Row],[AS_PATH_ACCESS_LIST]],as_path_access_list[NAME],as_path_access_list[LIST_NUMBER],""))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{F34C1CD3-F689-F243-A48C-8C2369C65715}" name="PREPEND"/>
-    <tableColumn id="10" xr3:uid="{1611BDA3-E9B5-9A43-9A8B-5AA2D76B0558}" name="AS" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{1611BDA3-E9B5-9A43-9A8B-5AA2D76B0558}" name="AS" dataDxfId="44">
       <calculatedColumnFormula>IF(ISBLANK(route_map[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(route_map[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{4983301E-AD3E-5E47-8601-4952DB168FF6}" name="LOCAL_PREFERENCE"/>
-    <tableColumn id="14" xr3:uid="{C744C15B-5995-5948-ABFC-C89B697A7FD5}" name="STATUS" dataDxfId="42"/>
+    <tableColumn id="14" xr3:uid="{C744C15B-5995-5948-ABFC-C89B697A7FD5}" name="STATUS" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F9E69226-D79B-E747-BF05-F20E7E3967F2}" name="bgp" displayName="bgp" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F9E69226-D79B-E747-BF05-F20E7E3967F2}" name="bgp" displayName="bgp" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="A1:G2" xr:uid="{F9E69226-D79B-E747-BF05-F20E7E3967F2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9A4B308A-0628-954A-8B73-E6B7E3F88611}" name="HOSTNAME" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{69095758-C320-E949-8693-7D8BC1B65999}" name="DEVICE_OS" dataDxfId="37">
+    <tableColumn id="1" xr3:uid="{9A4B308A-0628-954A-8B73-E6B7E3F88611}" name="HOSTNAME" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{69095758-C320-E949-8693-7D8BC1B65999}" name="DEVICE_OS" dataDxfId="38">
       <calculatedColumnFormula>IF(ISBLANK(bgp[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{C031DEF7-FB44-FA4C-816F-7A3195E36026}" name="VRF"/>
-    <tableColumn id="4" xr3:uid="{C08FBF8A-6212-A54D-BC50-A33BE246A13A}" name="AS" dataDxfId="36">
+    <tableColumn id="4" xr3:uid="{C08FBF8A-6212-A54D-BC50-A33BE246A13A}" name="AS" dataDxfId="37">
       <calculatedColumnFormula>IF(ISBLANK(bgp[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{6729EFFB-C388-934E-9275-E9DE3DE9149A}" name="BGP_ROUTER_ID" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{10E56D82-E692-B74D-8892-21AA9AEE5492}" name="MAXIMUM_PATHS" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{CCBECD29-7970-D643-884A-30AC44F2CA7B}" name="STATUS" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{6729EFFB-C388-934E-9275-E9DE3DE9149A}" name="BGP_ROUTER_ID" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{10E56D82-E692-B74D-8892-21AA9AEE5492}" name="MAXIMUM_PATHS" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{CCBECD29-7970-D643-884A-30AC44F2CA7B}" name="STATUS" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{63E7DFBB-8E9F-1B47-A4D4-8292B98E646B}" name="bgp_peer_session" displayName="bgp_peer_session" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{63E7DFBB-8E9F-1B47-A4D4-8292B98E646B}" name="bgp_peer_session" displayName="bgp_peer_session" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="A1:J2" xr:uid="{6AA3C6AA-A838-1F4C-B092-199D62D17036}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{87854EE4-6FC4-DF41-AB12-7D458E4020AE}" name="HOSTNAME" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{7D435938-004E-6A47-A13A-4654DFF65736}" name="DEVICE_OS" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{87854EE4-6FC4-DF41-AB12-7D458E4020AE}" name="HOSTNAME" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{7D435938-004E-6A47-A13A-4654DFF65736}" name="DEVICE_OS" dataDxfId="28">
       <calculatedColumnFormula>IF(ISBLANK(bgp_peer_session[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_peer_session[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F7A2993B-307E-1145-B768-0C0A7AD26B80}" name="NAME" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{F7A2993B-307E-1145-B768-0C0A7AD26B80}" name="NAME" dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{CA022A2B-7AF2-AD41-92A4-2ED8EB5C69BD}" name="UPDATE_SOURCE_LOOPBACK"/>
-    <tableColumn id="3" xr3:uid="{3C6B7608-B9E4-234A-B5BE-DB6EF22AD622}" name="LOOPBACK_ID" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{3C6B7608-B9E4-234A-B5BE-DB6EF22AD622}" name="LOOPBACK_ID" dataDxfId="26"/>
     <tableColumn id="4" xr3:uid="{DEB6A4A2-2145-B440-A898-597E6130F162}" name="REMOTE_AS"/>
-    <tableColumn id="6" xr3:uid="{A9901E50-F30C-6A42-981A-5DB5C0506332}" name="PASSWORD" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{A9901E50-F30C-6A42-981A-5DB5C0506332}" name="PASSWORD" dataDxfId="25"/>
     <tableColumn id="7" xr3:uid="{44A52967-D644-2A41-B57D-925F0D1F366A}" name="BFD"/>
-    <tableColumn id="8" xr3:uid="{3F42B443-71A0-2043-8087-FA49E25C73D4}" name="AS" dataDxfId="23">
+    <tableColumn id="8" xr3:uid="{3F42B443-71A0-2043-8087-FA49E25C73D4}" name="AS" dataDxfId="24">
       <calculatedColumnFormula>IF(ISBLANK(bgp_peer_session[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_peer_session[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B42417E9-0D0A-684C-B7A5-3ABD1026454E}" name="STATUS" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{B42417E9-0D0A-684C-B7A5-3ABD1026454E}" name="STATUS" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{23F9A1E1-54D9-044B-B6B6-74F9AC9A68F8}" name="bgp_peer_policy" displayName="bgp_peer_policy" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{23F9A1E1-54D9-044B-B6B6-74F9AC9A68F8}" name="bgp_peer_policy" displayName="bgp_peer_policy" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
   <autoFilter ref="A1:F2" xr:uid="{B83A0FB0-23B2-5148-A574-6F4D12FBD1EF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{669105BD-E395-0644-8B70-5D61530A9282}" name="HOSTNAME" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{4D5FB918-AD06-C247-ABDF-C01263E03CB8}" name="DEVICE_OS" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{669105BD-E395-0644-8B70-5D61530A9282}" name="HOSTNAME" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{4D5FB918-AD06-C247-ABDF-C01263E03CB8}" name="DEVICE_OS" dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(bgp_peer_policy[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_peer_policy[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{89A034EF-A08A-2A49-A4FF-D69F23183E1C}" name="NAME" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{966DC79E-2EB0-E44A-A0B6-63685C76559F}" name="OPTION" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{C22924C5-0B77-B142-8817-D37DB1442C4D}" name="AS" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{89A034EF-A08A-2A49-A4FF-D69F23183E1C}" name="NAME" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{966DC79E-2EB0-E44A-A0B6-63685C76559F}" name="OPTION" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{C22924C5-0B77-B142-8817-D37DB1442C4D}" name="AS" dataDxfId="16">
       <calculatedColumnFormula>IF(ISBLANK(bgp_peer_policy[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_peer_policy[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A09F5826-CE8C-8A46-8ADF-1D58B5DCAADE}" name="STATUS" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{A09F5826-CE8C-8A46-8ADF-1D58B5DCAADE}" name="STATUS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3865,11 +3878,11 @@
   <autoFilter ref="A1:T2" xr:uid="{40EE23F0-2330-3A44-B59F-2DD7161DAEF5}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{8F3E7A00-67CB-2B4A-A406-BCEE1724116E}" name="HOSTNAME"/>
-    <tableColumn id="13" xr3:uid="{E665B919-1AC8-854B-910F-1C7F14555272}" name="DEVICE_OS" dataDxfId="13">
+    <tableColumn id="13" xr3:uid="{E665B919-1AC8-854B-910F-1C7F14555272}" name="DEVICE_OS" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(bgp_neighbor[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_neighbor[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F3EA4101-30B4-1149-8CD4-09F0776F7A73}" name="VRF"/>
-    <tableColumn id="16" xr3:uid="{D4AFB5C2-8D00-E94D-A430-55427764BCCE}" name="AS" dataDxfId="12">
+    <tableColumn id="16" xr3:uid="{D4AFB5C2-8D00-E94D-A430-55427764BCCE}" name="AS" dataDxfId="13">
       <calculatedColumnFormula>IF(ISBLANK(bgp_neighbor[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_neighbor[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{162D1099-6F08-3646-8BFB-6E3695B938DB}" name="NEIGHBOR_IP_ADDRESS"/>
@@ -3878,8 +3891,8 @@
     <tableColumn id="7" xr3:uid="{E990F4DE-A2E2-FC4D-A924-4BA87A1D09A4}" name="PASSWORD"/>
     <tableColumn id="8" xr3:uid="{D92A002C-B002-BE4C-90D4-E83C376F3BE6}" name="BFD"/>
     <tableColumn id="9" xr3:uid="{37EA3139-01B6-BF45-9E46-BB1B3DD44865}" name="UPDATE_SOURCE_LOOPBACK"/>
-    <tableColumn id="10" xr3:uid="{45B22CF1-6556-7945-91E2-B5913A8899B1}" name="LOOPBACK_ID" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{DF0678A2-EFEF-B949-8925-FCA28C26F7D6}" name="INBOUND_ROUTE_MAP" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{45B22CF1-6556-7945-91E2-B5913A8899B1}" name="LOOPBACK_ID" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{DF0678A2-EFEF-B949-8925-FCA28C26F7D6}" name="INBOUND_ROUTE_MAP" dataDxfId="11"/>
     <tableColumn id="12" xr3:uid="{464983B4-142B-7F4F-8E97-2829FFDB1C85}" name="OUTBOUND_ROUTE_MAP"/>
     <tableColumn id="14" xr3:uid="{B870201F-9C4A-C844-9BF6-ABE50AF7A467}" name="LOCAL_AS"/>
     <tableColumn id="18" xr3:uid="{6DDC2C2B-7F23-DD44-A5CB-B445FD19D8FA}" name="BGP_PEER_SESSION_TEMPLATE"/>
@@ -3887,26 +3900,26 @@
     <tableColumn id="2" xr3:uid="{FD349F7D-E5B8-4AA7-81D8-FB0D3EB7F6B0}" name="ADVERTISE_MAP"/>
     <tableColumn id="3" xr3:uid="{EB74A2C5-7F63-4565-81BF-54E42781D618}" name="EXIST_MAP"/>
     <tableColumn id="20" xr3:uid="{325054A0-1849-494D-ADD6-D80FD71BB90D}" name="AS_OVERRIDE"/>
-    <tableColumn id="15" xr3:uid="{80838F91-9C40-E64E-9F83-E04B61C7C0E1}" name="STATUS" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{80838F91-9C40-E64E-9F83-E04B61C7C0E1}" name="STATUS" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CD5F5A88-B5B6-4A3B-8004-473D391B0469}" name="bgp_prefixes" displayName="bgp_prefixes" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CD5F5A88-B5B6-4A3B-8004-473D391B0469}" name="bgp_prefixes" displayName="bgp_prefixes" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A1:F2" xr:uid="{EAB2ADF2-E2DE-4951-AD17-B2B7E9D56A93}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7054123B-8A07-46DC-B660-B3A5D954CE13}" name="HOSTNAME" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{9E2F4E37-FF3F-3643-99A6-DED19D626976}" name="DEVICE_OS" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{7054123B-8A07-46DC-B660-B3A5D954CE13}" name="HOSTNAME" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{9E2F4E37-FF3F-3643-99A6-DED19D626976}" name="DEVICE_OS" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(bgp_prefixes[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_prefixes[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F78CE157-DD2A-4D20-BE23-A80A19C2A978}" name="VRF" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{DC27F453-12FA-4587-93AB-071F0D4C09A8}" name="AS" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{F78CE157-DD2A-4D20-BE23-A80A19C2A978}" name="VRF" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DC27F453-12FA-4587-93AB-071F0D4C09A8}" name="AS" dataDxfId="3">
       <calculatedColumnFormula>IF(ISBLANK(bgp_prefixes[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_prefixes[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{E581DD1B-5210-48F2-9ADB-3B0A3CB2EBBD}" name="PREFIX"/>
-    <tableColumn id="6" xr3:uid="{1C66C552-8D1A-534F-8103-25214087CAC6}" name="STATUS" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{1C66C552-8D1A-534F-8103-25214087CAC6}" name="STATUS" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3917,7 +3930,7 @@
   <autoFilter ref="A1:G2" xr:uid="{F5920AAD-CB6E-644A-B037-8E533DBDCE8E}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A38AE372-479B-6A43-BC48-283BCB211115}" name="HOSTNAME"/>
-    <tableColumn id="4" xr3:uid="{1071FC94-2FB8-436F-BB96-488968D4B5F2}" name="DEVICE_OS" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{1071FC94-2FB8-436F-BB96-488968D4B5F2}" name="DEVICE_OS" dataDxfId="1">
       <calculatedColumnFormula>IF(ISBLANK(rp[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(rp[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{6262426B-BCAA-934C-B149-85DA27DB04FC}" name="VRF"/>
@@ -3931,11 +3944,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D160ABCF-CDD5-F24F-B6E2-CC10F6567D78}" name="nxos_features" displayName="nxos_features" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="93" tableBorderDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D160ABCF-CDD5-F24F-B6E2-CC10F6567D78}" name="nxos_features" displayName="nxos_features" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="95" headerRowBorderDxfId="94" tableBorderDxfId="93">
   <autoFilter ref="A1:D2" xr:uid="{15558EBF-F85A-A54A-9CF1-6A04C78B7201}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8A2FA099-FDDE-0746-AE77-C7D431D3C178}" name="HOSTNAME"/>
-    <tableColumn id="2" xr3:uid="{087A5ABC-CC88-1343-9752-40ACB66DD53A}" name="DEVICE_OS" dataDxfId="91">
+    <tableColumn id="2" xr3:uid="{087A5ABC-CC88-1343-9752-40ACB66DD53A}" name="DEVICE_OS" dataDxfId="92">
       <calculatedColumnFormula>IF(ISBLANK(nxos_features[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(nxos_features[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{8877F4A4-A003-9449-8947-A98C70CE9643}" name="FEATURE"/>
@@ -3946,11 +3959,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1C28111F-59C8-6349-8EC8-6897FC5F5C3A}" name="port_channels" displayName="port_channels" ref="A1:H2" insertRow="1" totalsRowShown="0" tableBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1C28111F-59C8-6349-8EC8-6897FC5F5C3A}" name="port_channels" displayName="port_channels" ref="A1:H2" insertRow="1" totalsRowShown="0" tableBorderDxfId="91">
   <autoFilter ref="A1:H2" xr:uid="{CBC26200-4209-3849-9A7D-C5767C11C244}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7BAF873C-B8C3-E24E-AD51-5E071B2CEB26}" name="HOSTNAME"/>
-    <tableColumn id="2" xr3:uid="{259B4B4F-D29B-6F47-B76D-7BDDB5CFF220}" name="DEVICE_OS" dataDxfId="89">
+    <tableColumn id="2" xr3:uid="{259B4B4F-D29B-6F47-B76D-7BDDB5CFF220}" name="DEVICE_OS" dataDxfId="90">
       <calculatedColumnFormula>IF(ISBLANK(port_channels[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(port_channels[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{91FEB763-37C9-F54B-A3A9-5EE4EC230ED6}" name="INTERFACE"/>
@@ -3968,8 +3981,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DF33A378-F683-464D-B600-B63F32BDB3C9}" name="vrfs" displayName="vrfs" ref="A1:B2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{509D4756-A42E-114E-80F3-9D83D65AD5D8}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7FCF5EA8-1765-3940-8F7F-3D48D823D788}" name="NAME" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{942CE1F9-B9BF-F64E-8BF3-470081B77DDF}" name="RD" dataDxfId="87"/>
+    <tableColumn id="1" xr3:uid="{7FCF5EA8-1765-3940-8F7F-3D48D823D788}" name="NAME" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{942CE1F9-B9BF-F64E-8BF3-470081B77DDF}" name="RD" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3980,11 +3993,11 @@
   <autoFilter ref="A1:H2" xr:uid="{A1F75A44-21CF-004B-8425-2DD34E03999C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{706BFCCC-5CCB-DA44-9DF3-112D9FC3BA05}" name="HOSTNAME"/>
-    <tableColumn id="3" xr3:uid="{1615B641-38A5-F84C-B425-C5C2B0A97AD5}" name="DEVICE_OS" dataDxfId="86">
+    <tableColumn id="3" xr3:uid="{1615B641-38A5-F84C-B425-C5C2B0A97AD5}" name="DEVICE_OS" dataDxfId="87">
       <calculatedColumnFormula>IF(ISBLANK(device_vrfs[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(device_vrfs[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{45F93218-1BB6-844A-9CA4-DD101878B936}" name="VRF"/>
-    <tableColumn id="7" xr3:uid="{AEF4F533-EA19-6749-9BBA-6A212F98D99A}" name="RD" dataDxfId="85">
+    <tableColumn id="7" xr3:uid="{AEF4F533-EA19-6749-9BBA-6A212F98D99A}" name="RD" dataDxfId="86">
       <calculatedColumnFormula>IF(ISBLANK(device_vrfs[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(device_vrfs[[#This Row],[VRF]],vrfs[NAME],vrfs[RD]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{21AD3C2D-D1E0-814C-BCBF-C1AEF70A40EE}" name="DESCRIPTION"/>
@@ -4001,13 +4014,13 @@
   <autoFilter ref="A1:G2" xr:uid="{C3970CA1-6E2C-C447-9BFB-1AB7967FF334}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E67AA695-2B32-D945-BD4F-1666452C64C8}" name="HOSTNAME"/>
-    <tableColumn id="4" xr3:uid="{FD19EBAC-CB04-0A40-BA8B-D0BE4CCBBA41}" name="DEVICE_OS" dataDxfId="84">
+    <tableColumn id="4" xr3:uid="{FD19EBAC-CB04-0A40-BA8B-D0BE4CCBBA41}" name="DEVICE_OS" dataDxfId="85">
       <calculatedColumnFormula>IF(ISBLANK(ospf[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(ospf[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{D3C42C66-3DA0-3748-88FC-46126DD845FF}" name="VRF"/>
     <tableColumn id="18" xr3:uid="{D649DB6A-A0F0-2A4B-AC4F-2445F55575AD}" name="OSPF_ID"/>
-    <tableColumn id="19" xr3:uid="{A6FA7A3A-EA03-7146-A1C7-2B2F831A7326}" name="OSPF_ROUTER_ID" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{EF667B63-5704-1541-A7A0-DAECF2E40AE8}" name="REFERENCE_BANDWIDTH" dataDxfId="82"/>
+    <tableColumn id="19" xr3:uid="{A6FA7A3A-EA03-7146-A1C7-2B2F831A7326}" name="OSPF_ROUTER_ID" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{EF667B63-5704-1541-A7A0-DAECF2E40AE8}" name="REFERENCE_BANDWIDTH" dataDxfId="83"/>
     <tableColumn id="9" xr3:uid="{22492105-FDAF-C54C-8187-669D12E64D0D}" name="STATUS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4020,13 +4033,13 @@
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{1745545E-5B6E-7345-A78B-D6204938F96E}" name="HOSTNAME"/>
     <tableColumn id="2" xr3:uid="{D3B63833-3EC7-7646-BE68-0F336F6461FC}" name="VRF"/>
-    <tableColumn id="7" xr3:uid="{249A88F6-760F-4F77-B377-DE8FEE13454F}" name="DEVICE_OS" dataDxfId="81">
+    <tableColumn id="7" xr3:uid="{249A88F6-760F-4F77-B377-DE8FEE13454F}" name="DEVICE_OS" dataDxfId="82">
       <calculatedColumnFormula>IF(ISBLANK(loopbacks[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(loopbacks[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{CF28568B-30CB-9A4C-84A0-65AD2F529CD9}" name="LO_ID"/>
-    <tableColumn id="4" xr3:uid="{80D1A26E-FA76-D74E-8315-DD3C64461A10}" name="IP_ADDRESS" dataDxfId="80"/>
-    <tableColumn id="14" xr3:uid="{363298CE-69B3-864C-9214-74A6B5AB7141}" name="ENABLE_OSPF" dataDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{FBE12430-F154-7243-A2C6-4C583194D3F8}" name="OSPF_ID" dataDxfId="78">
+    <tableColumn id="4" xr3:uid="{80D1A26E-FA76-D74E-8315-DD3C64461A10}" name="IP_ADDRESS" dataDxfId="81"/>
+    <tableColumn id="14" xr3:uid="{363298CE-69B3-864C-9214-74A6B5AB7141}" name="ENABLE_OSPF" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{FBE12430-F154-7243-A2C6-4C583194D3F8}" name="OSPF_ID" dataDxfId="79">
       <calculatedColumnFormula array="1">IF(loopbacks[[#This Row],[ENABLE_OSPF]] = "No","",_xlfn.XLOOKUP(_xlfn.SINGLE(loopbacks[HOSTNAME])&amp;loopbacks[[#This Row],[VRF]],ospf[HOSTNAME]&amp;ospf[VRF],ospf[OSPF_ID]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{175A7AB2-1C5C-A549-B557-5E248E423806}" name="OSPF_AREA"/>
@@ -4044,10 +4057,10 @@
   <autoFilter ref="A1:W2" xr:uid="{DD216AC4-FD74-6E47-B4CC-3F9FC894EFFD}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{1FBD31D9-874E-AF4E-A3D1-141126E87D87}" name="HOSTNAME"/>
-    <tableColumn id="2" xr3:uid="{C3A2D69F-5FE5-D345-9794-E2ED301C4D34}" name="DEVICE_OS" dataDxfId="77">
+    <tableColumn id="2" xr3:uid="{C3A2D69F-5FE5-D345-9794-E2ED301C4D34}" name="DEVICE_OS" dataDxfId="78">
       <calculatedColumnFormula>IF(ISBLANK(interfaces[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(interfaces[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{B104D4FB-806E-EF4E-BC7A-5368F78F484C}" name="DEVICE_TYPE" dataDxfId="76">
+    <tableColumn id="24" xr3:uid="{B104D4FB-806E-EF4E-BC7A-5368F78F484C}" name="DEVICE_TYPE" dataDxfId="77">
       <calculatedColumnFormula>IF(ISBLANK(interfaces[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(interfaces[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_TYPE]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{C130E233-5749-9C41-8467-517B8E4098A0}" name="INTERFACE"/>
@@ -4055,7 +4068,7 @@
     <tableColumn id="5" xr3:uid="{62E47652-D42D-9247-A7EF-78ECEE9BD10E}" name="VRF"/>
     <tableColumn id="13" xr3:uid="{E2CE50A5-8FCC-5945-A33E-490E37B5B251}" name="IP_ADDRESS"/>
     <tableColumn id="6" xr3:uid="{D72F0F76-AFC8-5A40-A52D-7C082916411E}" name="ENABLE_OSPF"/>
-    <tableColumn id="7" xr3:uid="{F0FDD87C-D7F7-C94C-9554-C131A9109A26}" name="OSPF_ID" dataDxfId="75">
+    <tableColumn id="7" xr3:uid="{F0FDD87C-D7F7-C94C-9554-C131A9109A26}" name="OSPF_ID" dataDxfId="76">
       <calculatedColumnFormula array="1">IF(interfaces[[#This Row],[ENABLE_OSPF]] = "No","",_xlfn.XLOOKUP(_xlfn.SINGLE(interfaces[HOSTNAME])&amp;interfaces[[#This Row],[VRF]],ospf[HOSTNAME]&amp;ospf[VRF],ospf[OSPF_ID]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{249B22EF-515D-C242-810D-1ADBEF5DCACC}" name="OSPF_AREA"/>
@@ -4078,26 +4091,26 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{EF182424-B364-2E40-B9E7-2D19AD52806B}" name="as_path_access_list" displayName="as_path_access_list" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{EF182424-B364-2E40-B9E7-2D19AD52806B}" name="as_path_access_list" displayName="as_path_access_list" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74">
   <autoFilter ref="A1:H2" xr:uid="{46C7A6E1-AD48-0148-8EAE-A397341A8F27}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{95E55C61-E799-7E4C-87D2-32EB02EDF339}" name="HOSTNAME" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{0260098B-0476-9F49-96A3-CFF841B40E86}" name="DEVICE_OS" dataDxfId="70">
+    <tableColumn id="1" xr3:uid="{95E55C61-E799-7E4C-87D2-32EB02EDF339}" name="HOSTNAME" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{0260098B-0476-9F49-96A3-CFF841B40E86}" name="DEVICE_OS" dataDxfId="71">
       <calculatedColumnFormula>IF(ISBLANK(as_path_access_list[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(as_path_access_list[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8D31D796-4B4A-D547-9FBD-4199CC9BE96F}" name="NAME" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{76DD162F-BE3A-A446-8FFF-A1BBEE98D558}" name="LIST_NUMBER" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{C7FA814C-3D8C-4C46-A361-F3B427EF7CEC}" name="SEQUENCE" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{6D448DBA-7BE6-A24B-94B2-F8F9DC0D5202}" name="ACTION" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{D745686C-80DD-7B4B-B1EB-891B99684EE6}" name="REGULAR_EXPRESSION" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{86F6B4B2-27A7-C648-BBA6-A86FB7BA76CE}" name="STATUS" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{8D31D796-4B4A-D547-9FBD-4199CC9BE96F}" name="NAME" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{76DD162F-BE3A-A446-8FFF-A1BBEE98D558}" name="LIST_NUMBER" dataDxfId="69"/>
+    <tableColumn id="9" xr3:uid="{C7FA814C-3D8C-4C46-A361-F3B427EF7CEC}" name="SEQUENCE" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{6D448DBA-7BE6-A24B-94B2-F8F9DC0D5202}" name="ACTION" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{D745686C-80DD-7B4B-B1EB-891B99684EE6}" name="REGULAR_EXPRESSION" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{86F6B4B2-27A7-C648-BBA6-A86FB7BA76CE}" name="STATUS" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4385,7 +4398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4401,10 +4414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A47D4A-1E9B-EF4E-8065-17402CAF3208}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <selection activeCell="I8" sqref="I8:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4417,12 +4430,13 @@
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4448,40 +4462,44 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>449</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="G2" s="19"/>
       <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{41FB4655-EBF7-814C-8C99-FE684AC3E8AE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{41FB4655-EBF7-814C-8C99-FE684AC3E8AE}">
       <formula1>"present,ignored"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updating the excel file to support QoS
</commit_message>
<xml_diff>
--- a/spreadsheets/ipn.xlsx
+++ b/spreadsheets/ipn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calange/PycharmProjects/ipn_isn_automation/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6467F20-2907-A34C-9B3E-8C1FD571C5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940AFCF1-2EEB-4D40-A676-FC0093E606E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15700" yWindow="-28800" windowWidth="68800" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15700" yWindow="-28800" windowWidth="68800" windowHeight="28800" firstSheet="2" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,11 @@
     <sheet name="bgp_neighbor" sheetId="11" r:id="rId15"/>
     <sheet name="bgp_prefixes" sheetId="17" r:id="rId16"/>
     <sheet name="rp" sheetId="23" r:id="rId17"/>
-    <sheet name="Source" sheetId="10" r:id="rId18"/>
+    <sheet name="class_map_qos" sheetId="25" r:id="rId18"/>
+    <sheet name="policy_map_qos" sheetId="26" r:id="rId19"/>
+    <sheet name="policy_map_queuing" sheetId="27" r:id="rId20"/>
+    <sheet name="system_qos_queuing_output" sheetId="28" r:id="rId21"/>
+    <sheet name="Source" sheetId="10" r:id="rId22"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">devices_vrfs!$A$1:$D$2</definedName>
@@ -43,6 +47,7 @@
     <definedName name="IOS_XR">Source!$B$2:$B$20</definedName>
     <definedName name="NEXUS">Source!$E$2:$E$66</definedName>
     <definedName name="NXOS">Source!$E:$E</definedName>
+    <definedName name="policy_map_queuing_name">policy_map_queuing[NAME]</definedName>
     <definedName name="XR">Source!$B$2:$B$8</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -101,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="457">
   <si>
     <t>HOSTNAME</t>
   </si>
@@ -1451,6 +1456,27 @@
   </si>
   <si>
     <t>MGMT_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>MATCH</t>
+  </si>
+  <si>
+    <t>MATCH_VALUE</t>
+  </si>
+  <si>
+    <t>CLASS_MAP_NAME</t>
+  </si>
+  <si>
+    <t>QOS_GROUP</t>
+  </si>
+  <si>
+    <t>QUEUING</t>
+  </si>
+  <si>
+    <t>PRIORITY_LEVEL</t>
+  </si>
+  <si>
+    <t>BANDWIDTH</t>
   </si>
 </sst>
 </file>
@@ -1555,7 +1581,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1634,12 +1660,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF8EA9DB"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1662,12 +1714,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{7E5BFF21-FF29-42C5-8362-8040CB29CF6C}"/>
   </cellStyles>
-  <dxfs count="101">
+  <dxfs count="116">
     <dxf>
       <font>
         <b val="0"/>
@@ -1680,11 +1734,292 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3643,6 +3978,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <border outline="0">
         <left style="thin">
           <color theme="4" tint="-0.24994659260841701"/>
@@ -3739,15 +4092,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{509596C7-D353-D14A-BD3B-3A0CCF6D18AE}" name="devices" displayName="devices" ref="A1:Q2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:Q2" xr:uid="{6F3A0D7A-D722-E743-99ED-9A12FCB8C763}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{381CC9EE-E379-3949-8A0B-9662994EC61F}" name="HOSTNAME" dataDxfId="100"/>
-    <tableColumn id="16" xr3:uid="{D41A0F4C-32E3-DC40-BE24-4D9B419C9A57}" name="SERIAL_NUMBER" dataDxfId="99"/>
+    <tableColumn id="1" xr3:uid="{381CC9EE-E379-3949-8A0B-9662994EC61F}" name="HOSTNAME" dataDxfId="115"/>
+    <tableColumn id="16" xr3:uid="{D41A0F4C-32E3-DC40-BE24-4D9B419C9A57}" name="SERIAL_NUMBER" dataDxfId="114"/>
     <tableColumn id="2" xr3:uid="{DF76891E-9FEE-364E-950B-D2AF1487DE91}" name="DEVICE_OS"/>
     <tableColumn id="7" xr3:uid="{599A17A7-36B0-5E42-BB84-35BAA37040F9}" name="DEVICE_TYPE"/>
     <tableColumn id="3" xr3:uid="{CB026E15-2101-8E49-B5EA-A19D5EA278E1}" name="MGMT_INT"/>
-    <tableColumn id="4" xr3:uid="{10B5AEE1-2F46-8140-80E7-23A7CF06F12B}" name="MGMT_VRF" dataDxfId="98"/>
-    <tableColumn id="5" xr3:uid="{8E625E2F-DFC3-1E47-9623-DFDC9AA7CC26}" name="MGMT_IP" dataDxfId="97"/>
-    <tableColumn id="6" xr3:uid="{381A8401-24A4-7F45-8DCA-CA9B15CACEA9}" name="MGMT_GW" dataDxfId="96"/>
-    <tableColumn id="17" xr3:uid="{107D9780-9B12-CC4B-8637-1943D81E2D2E}" name="MGMT_DESCRIPTION" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{10B5AEE1-2F46-8140-80E7-23A7CF06F12B}" name="MGMT_VRF" dataDxfId="113"/>
+    <tableColumn id="5" xr3:uid="{8E625E2F-DFC3-1E47-9623-DFDC9AA7CC26}" name="MGMT_IP" dataDxfId="112"/>
+    <tableColumn id="6" xr3:uid="{381A8401-24A4-7F45-8DCA-CA9B15CACEA9}" name="MGMT_GW" dataDxfId="111"/>
+    <tableColumn id="17" xr3:uid="{107D9780-9B12-CC4B-8637-1943D81E2D2E}" name="MGMT_DESCRIPTION" dataDxfId="110"/>
     <tableColumn id="8" xr3:uid="{FD91D019-1042-1A4B-9C02-3E16ECD3C6B8}" name="USERNAME"/>
     <tableColumn id="9" xr3:uid="{9016DBD0-0BD9-B44A-87D7-39611823CBC1}" name="PASSWORD"/>
     <tableColumn id="10" xr3:uid="{7BDC3620-DB6A-ED45-B7EF-A52B60E5A63A}" name="ENABLE"/>
@@ -3762,33 +4115,33 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{66160081-DEC2-404A-B86C-A5A1FE0E2385}" name="prefix_list" displayName="prefix_list" ref="A1:K2" insertRow="1" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{66160081-DEC2-404A-B86C-A5A1FE0E2385}" name="prefix_list" displayName="prefix_list" ref="A1:K2" insertRow="1" totalsRowShown="0" headerRowDxfId="78" dataDxfId="76" headerRowBorderDxfId="77" tableBorderDxfId="75" totalsRowBorderDxfId="74">
   <autoFilter ref="A1:K2" xr:uid="{D55CF0F7-6E4A-BF4C-918F-5A724EA4861F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F2D78B99-533C-B649-93FC-1E9C4AF83F80}" name="HOSTNAME" dataDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{17B5652C-C4F7-004A-8AF1-BABF5656C432}" name="DEVICE_OS" dataDxfId="58">
+    <tableColumn id="1" xr3:uid="{F2D78B99-533C-B649-93FC-1E9C4AF83F80}" name="HOSTNAME" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{17B5652C-C4F7-004A-8AF1-BABF5656C432}" name="DEVICE_OS" dataDxfId="72">
       <calculatedColumnFormula>IF(ISBLANK(prefix_list[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(prefix_list[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F9A61C22-2FDA-A642-AA1F-8E9A458C6039}" name="NAME" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{1C364EF9-1AFD-2D4B-B61D-1591B410DD90}" name="DESCRIPTION" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{35AA2362-D924-F44C-B2F2-40764BA64F59}" name="ADDRESS_FAMILY" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{88DA9E15-E49F-1849-9616-0F4813B909F5}" name="SEQUENCE" dataDxfId="54"/>
-    <tableColumn id="7" xr3:uid="{9296DC93-138E-114B-81F3-49030054A86C}" name="ACTION" dataDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{9FF719D3-00E1-634D-8391-AD1803B05B20}" name="PREFIX" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{D1D60C28-AF41-5F4F-ABB6-02186395F57B}" name="GE" dataDxfId="51"/>
-    <tableColumn id="10" xr3:uid="{1E602C71-DB91-C04B-912A-1D1DDE852D43}" name="LE" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{5BCFBE35-DC23-4440-884F-5291013B2AD8}" name="STATUS" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{F9A61C22-2FDA-A642-AA1F-8E9A458C6039}" name="NAME" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{1C364EF9-1AFD-2D4B-B61D-1591B410DD90}" name="DESCRIPTION" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{35AA2362-D924-F44C-B2F2-40764BA64F59}" name="ADDRESS_FAMILY" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{88DA9E15-E49F-1849-9616-0F4813B909F5}" name="SEQUENCE" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{9296DC93-138E-114B-81F3-49030054A86C}" name="ACTION" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{9FF719D3-00E1-634D-8391-AD1803B05B20}" name="PREFIX" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{D1D60C28-AF41-5F4F-ABB6-02186395F57B}" name="GE" dataDxfId="65"/>
+    <tableColumn id="10" xr3:uid="{1E602C71-DB91-C04B-912A-1D1DDE852D43}" name="LE" dataDxfId="64"/>
+    <tableColumn id="11" xr3:uid="{5BCFBE35-DC23-4440-884F-5291013B2AD8}" name="STATUS" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6E452009-DEEF-5C4C-85C0-8D759B63A698}" name="route_map" displayName="route_map" ref="A1:M2" insertRow="1" totalsRowShown="0" tableBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6E452009-DEEF-5C4C-85C0-8D759B63A698}" name="route_map" displayName="route_map" ref="A1:M2" insertRow="1" totalsRowShown="0" tableBorderDxfId="62">
   <autoFilter ref="A1:M2" xr:uid="{97EDB19E-68E0-B14D-837F-27C451B5CB8C}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{3BDEDE97-72E9-C84A-9F44-E18054506FE4}" name="HOSTNAME" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{7506AE33-5FAA-044A-8B2B-E417F16E93C8}" name="DEVICE_OS" dataDxfId="46">
+    <tableColumn id="1" xr3:uid="{3BDEDE97-72E9-C84A-9F44-E18054506FE4}" name="HOSTNAME" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{7506AE33-5FAA-044A-8B2B-E417F16E93C8}" name="DEVICE_OS" dataDxfId="60">
       <calculatedColumnFormula>IF(ISBLANK(route_map[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(route_map[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{1F665B2D-B35E-FC4D-9C4C-B9595DC2D3F7}" name="NAME"/>
@@ -3797,77 +4150,77 @@
     <tableColumn id="5" xr3:uid="{91A7A709-9BA1-4743-BFBA-C980FCA55C61}" name="ACTION"/>
     <tableColumn id="6" xr3:uid="{37FEFFEE-58D5-BF47-A6AC-D4DB9D9CD4EC}" name="PREFIX_LIST"/>
     <tableColumn id="7" xr3:uid="{089E8480-CD75-2F45-93E1-67BA2B42FF21}" name="AS_PATH_ACCESS_LIST"/>
-    <tableColumn id="8" xr3:uid="{F9459908-C24B-9144-8097-1F11F1CB8FFA}" name="AS_PATH_ACCESS_LIST_NUMBER" dataDxfId="45">
+    <tableColumn id="8" xr3:uid="{F9459908-C24B-9144-8097-1F11F1CB8FFA}" name="AS_PATH_ACCESS_LIST_NUMBER" dataDxfId="59">
       <calculatedColumnFormula>IF(ISBLANK(route_map[[#This Row],[AS_PATH_ACCESS_LIST]]),"",_xlfn.XLOOKUP(route_map[[#This Row],[AS_PATH_ACCESS_LIST]],as_path_access_list[NAME],as_path_access_list[LIST_NUMBER],""))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{F34C1CD3-F689-F243-A48C-8C2369C65715}" name="PREPEND"/>
-    <tableColumn id="10" xr3:uid="{1611BDA3-E9B5-9A43-9A8B-5AA2D76B0558}" name="AS" dataDxfId="44">
+    <tableColumn id="10" xr3:uid="{1611BDA3-E9B5-9A43-9A8B-5AA2D76B0558}" name="AS" dataDxfId="58">
       <calculatedColumnFormula>IF(ISBLANK(route_map[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(route_map[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{4983301E-AD3E-5E47-8601-4952DB168FF6}" name="LOCAL_PREFERENCE"/>
-    <tableColumn id="14" xr3:uid="{C744C15B-5995-5948-ABFC-C89B697A7FD5}" name="STATUS" dataDxfId="43"/>
+    <tableColumn id="14" xr3:uid="{C744C15B-5995-5948-ABFC-C89B697A7FD5}" name="STATUS" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F9E69226-D79B-E747-BF05-F20E7E3967F2}" name="bgp" displayName="bgp" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{F9E69226-D79B-E747-BF05-F20E7E3967F2}" name="bgp" displayName="bgp" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54">
   <autoFilter ref="A1:G2" xr:uid="{F9E69226-D79B-E747-BF05-F20E7E3967F2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9A4B308A-0628-954A-8B73-E6B7E3F88611}" name="HOSTNAME" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{69095758-C320-E949-8693-7D8BC1B65999}" name="DEVICE_OS" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{9A4B308A-0628-954A-8B73-E6B7E3F88611}" name="HOSTNAME" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{69095758-C320-E949-8693-7D8BC1B65999}" name="DEVICE_OS" dataDxfId="52">
       <calculatedColumnFormula>IF(ISBLANK(bgp[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{C031DEF7-FB44-FA4C-816F-7A3195E36026}" name="VRF"/>
-    <tableColumn id="4" xr3:uid="{C08FBF8A-6212-A54D-BC50-A33BE246A13A}" name="AS" dataDxfId="37">
+    <tableColumn id="4" xr3:uid="{C08FBF8A-6212-A54D-BC50-A33BE246A13A}" name="AS" dataDxfId="51">
       <calculatedColumnFormula>IF(ISBLANK(bgp[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{6729EFFB-C388-934E-9275-E9DE3DE9149A}" name="BGP_ROUTER_ID" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{10E56D82-E692-B74D-8892-21AA9AEE5492}" name="MAXIMUM_PATHS" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{CCBECD29-7970-D643-884A-30AC44F2CA7B}" name="STATUS" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{6729EFFB-C388-934E-9275-E9DE3DE9149A}" name="BGP_ROUTER_ID" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{10E56D82-E692-B74D-8892-21AA9AEE5492}" name="MAXIMUM_PATHS" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{CCBECD29-7970-D643-884A-30AC44F2CA7B}" name="STATUS" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{63E7DFBB-8E9F-1B47-A4D4-8292B98E646B}" name="bgp_peer_session" displayName="bgp_peer_session" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{63E7DFBB-8E9F-1B47-A4D4-8292B98E646B}" name="bgp_peer_session" displayName="bgp_peer_session" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <autoFilter ref="A1:J2" xr:uid="{6AA3C6AA-A838-1F4C-B092-199D62D17036}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{87854EE4-6FC4-DF41-AB12-7D458E4020AE}" name="HOSTNAME" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{7D435938-004E-6A47-A13A-4654DFF65736}" name="DEVICE_OS" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{87854EE4-6FC4-DF41-AB12-7D458E4020AE}" name="HOSTNAME" dataDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{7D435938-004E-6A47-A13A-4654DFF65736}" name="DEVICE_OS" dataDxfId="42">
       <calculatedColumnFormula>IF(ISBLANK(bgp_peer_session[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_peer_session[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F7A2993B-307E-1145-B768-0C0A7AD26B80}" name="NAME" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{F7A2993B-307E-1145-B768-0C0A7AD26B80}" name="NAME" dataDxfId="41"/>
     <tableColumn id="2" xr3:uid="{CA022A2B-7AF2-AD41-92A4-2ED8EB5C69BD}" name="UPDATE_SOURCE_LOOPBACK"/>
-    <tableColumn id="3" xr3:uid="{3C6B7608-B9E4-234A-B5BE-DB6EF22AD622}" name="LOOPBACK_ID" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{3C6B7608-B9E4-234A-B5BE-DB6EF22AD622}" name="LOOPBACK_ID" dataDxfId="40"/>
     <tableColumn id="4" xr3:uid="{DEB6A4A2-2145-B440-A898-597E6130F162}" name="REMOTE_AS"/>
-    <tableColumn id="6" xr3:uid="{A9901E50-F30C-6A42-981A-5DB5C0506332}" name="PASSWORD" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{A9901E50-F30C-6A42-981A-5DB5C0506332}" name="PASSWORD" dataDxfId="39"/>
     <tableColumn id="7" xr3:uid="{44A52967-D644-2A41-B57D-925F0D1F366A}" name="BFD"/>
-    <tableColumn id="8" xr3:uid="{3F42B443-71A0-2043-8087-FA49E25C73D4}" name="AS" dataDxfId="24">
+    <tableColumn id="8" xr3:uid="{3F42B443-71A0-2043-8087-FA49E25C73D4}" name="AS" dataDxfId="38">
       <calculatedColumnFormula>IF(ISBLANK(bgp_peer_session[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_peer_session[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B42417E9-0D0A-684C-B7A5-3ABD1026454E}" name="STATUS" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{B42417E9-0D0A-684C-B7A5-3ABD1026454E}" name="STATUS" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{23F9A1E1-54D9-044B-B6B6-74F9AC9A68F8}" name="bgp_peer_policy" displayName="bgp_peer_policy" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{23F9A1E1-54D9-044B-B6B6-74F9AC9A68F8}" name="bgp_peer_policy" displayName="bgp_peer_policy" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="36" tableBorderDxfId="35">
   <autoFilter ref="A1:F2" xr:uid="{B83A0FB0-23B2-5148-A574-6F4D12FBD1EF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{669105BD-E395-0644-8B70-5D61530A9282}" name="HOSTNAME" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{4D5FB918-AD06-C247-ABDF-C01263E03CB8}" name="DEVICE_OS" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{669105BD-E395-0644-8B70-5D61530A9282}" name="HOSTNAME" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{4D5FB918-AD06-C247-ABDF-C01263E03CB8}" name="DEVICE_OS" dataDxfId="33">
       <calculatedColumnFormula>IF(ISBLANK(bgp_peer_policy[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_peer_policy[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{89A034EF-A08A-2A49-A4FF-D69F23183E1C}" name="NAME" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{966DC79E-2EB0-E44A-A0B6-63685C76559F}" name="OPTION" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{C22924C5-0B77-B142-8817-D37DB1442C4D}" name="AS" dataDxfId="16">
+    <tableColumn id="2" xr3:uid="{89A034EF-A08A-2A49-A4FF-D69F23183E1C}" name="NAME" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{966DC79E-2EB0-E44A-A0B6-63685C76559F}" name="OPTION" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{C22924C5-0B77-B142-8817-D37DB1442C4D}" name="AS" dataDxfId="30">
       <calculatedColumnFormula>IF(ISBLANK(bgp_peer_policy[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_peer_policy[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A09F5826-CE8C-8A46-8ADF-1D58B5DCAADE}" name="STATUS" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{A09F5826-CE8C-8A46-8ADF-1D58B5DCAADE}" name="STATUS" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3878,11 +4231,11 @@
   <autoFilter ref="A1:T2" xr:uid="{40EE23F0-2330-3A44-B59F-2DD7161DAEF5}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{8F3E7A00-67CB-2B4A-A406-BCEE1724116E}" name="HOSTNAME"/>
-    <tableColumn id="13" xr3:uid="{E665B919-1AC8-854B-910F-1C7F14555272}" name="DEVICE_OS" dataDxfId="14">
+    <tableColumn id="13" xr3:uid="{E665B919-1AC8-854B-910F-1C7F14555272}" name="DEVICE_OS" dataDxfId="28">
       <calculatedColumnFormula>IF(ISBLANK(bgp_neighbor[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_neighbor[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F3EA4101-30B4-1149-8CD4-09F0776F7A73}" name="VRF"/>
-    <tableColumn id="16" xr3:uid="{D4AFB5C2-8D00-E94D-A430-55427764BCCE}" name="AS" dataDxfId="13">
+    <tableColumn id="16" xr3:uid="{D4AFB5C2-8D00-E94D-A430-55427764BCCE}" name="AS" dataDxfId="27">
       <calculatedColumnFormula>IF(ISBLANK(bgp_neighbor[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_neighbor[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{162D1099-6F08-3646-8BFB-6E3695B938DB}" name="NEIGHBOR_IP_ADDRESS"/>
@@ -3891,8 +4244,8 @@
     <tableColumn id="7" xr3:uid="{E990F4DE-A2E2-FC4D-A924-4BA87A1D09A4}" name="PASSWORD"/>
     <tableColumn id="8" xr3:uid="{D92A002C-B002-BE4C-90D4-E83C376F3BE6}" name="BFD"/>
     <tableColumn id="9" xr3:uid="{37EA3139-01B6-BF45-9E46-BB1B3DD44865}" name="UPDATE_SOURCE_LOOPBACK"/>
-    <tableColumn id="10" xr3:uid="{45B22CF1-6556-7945-91E2-B5913A8899B1}" name="LOOPBACK_ID" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{DF0678A2-EFEF-B949-8925-FCA28C26F7D6}" name="INBOUND_ROUTE_MAP" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{45B22CF1-6556-7945-91E2-B5913A8899B1}" name="LOOPBACK_ID" dataDxfId="26"/>
+    <tableColumn id="11" xr3:uid="{DF0678A2-EFEF-B949-8925-FCA28C26F7D6}" name="INBOUND_ROUTE_MAP" dataDxfId="25"/>
     <tableColumn id="12" xr3:uid="{464983B4-142B-7F4F-8E97-2829FFDB1C85}" name="OUTBOUND_ROUTE_MAP"/>
     <tableColumn id="14" xr3:uid="{B870201F-9C4A-C844-9BF6-ABE50AF7A467}" name="LOCAL_AS"/>
     <tableColumn id="18" xr3:uid="{6DDC2C2B-7F23-DD44-A5CB-B445FD19D8FA}" name="BGP_PEER_SESSION_TEMPLATE"/>
@@ -3900,26 +4253,26 @@
     <tableColumn id="2" xr3:uid="{FD349F7D-E5B8-4AA7-81D8-FB0D3EB7F6B0}" name="ADVERTISE_MAP"/>
     <tableColumn id="3" xr3:uid="{EB74A2C5-7F63-4565-81BF-54E42781D618}" name="EXIST_MAP"/>
     <tableColumn id="20" xr3:uid="{325054A0-1849-494D-ADD6-D80FD71BB90D}" name="AS_OVERRIDE"/>
-    <tableColumn id="15" xr3:uid="{80838F91-9C40-E64E-9F83-E04B61C7C0E1}" name="STATUS" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{80838F91-9C40-E64E-9F83-E04B61C7C0E1}" name="STATUS" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CD5F5A88-B5B6-4A3B-8004-473D391B0469}" name="bgp_prefixes" displayName="bgp_prefixes" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CD5F5A88-B5B6-4A3B-8004-473D391B0469}" name="bgp_prefixes" displayName="bgp_prefixes" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21">
   <autoFilter ref="A1:F2" xr:uid="{EAB2ADF2-E2DE-4951-AD17-B2B7E9D56A93}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7054123B-8A07-46DC-B660-B3A5D954CE13}" name="HOSTNAME" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{9E2F4E37-FF3F-3643-99A6-DED19D626976}" name="DEVICE_OS" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{7054123B-8A07-46DC-B660-B3A5D954CE13}" name="HOSTNAME" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{9E2F4E37-FF3F-3643-99A6-DED19D626976}" name="DEVICE_OS" dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(bgp_prefixes[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_prefixes[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F78CE157-DD2A-4D20-BE23-A80A19C2A978}" name="VRF" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{DC27F453-12FA-4587-93AB-071F0D4C09A8}" name="AS" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{F78CE157-DD2A-4D20-BE23-A80A19C2A978}" name="VRF" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{DC27F453-12FA-4587-93AB-071F0D4C09A8}" name="AS" dataDxfId="17">
       <calculatedColumnFormula>IF(ISBLANK(bgp_prefixes[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(bgp_prefixes[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[ASN]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{E581DD1B-5210-48F2-9ADB-3B0A3CB2EBBD}" name="PREFIX"/>
-    <tableColumn id="6" xr3:uid="{1C66C552-8D1A-534F-8103-25214087CAC6}" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{1C66C552-8D1A-534F-8103-25214087CAC6}" name="STATUS" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3930,7 +4283,7 @@
   <autoFilter ref="A1:G2" xr:uid="{F5920AAD-CB6E-644A-B037-8E533DBDCE8E}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A38AE372-479B-6A43-BC48-283BCB211115}" name="HOSTNAME"/>
-    <tableColumn id="4" xr3:uid="{1071FC94-2FB8-436F-BB96-488968D4B5F2}" name="DEVICE_OS" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{1071FC94-2FB8-436F-BB96-488968D4B5F2}" name="DEVICE_OS" dataDxfId="15">
       <calculatedColumnFormula>IF(ISBLANK(rp[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(rp[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{6262426B-BCAA-934C-B149-85DA27DB04FC}" name="VRF"/>
@@ -3943,12 +4296,40 @@
 </table>
 </file>
 
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{99A6AB2F-E55E-504E-B11A-162B09601887}" name="class_map_qos" displayName="class_map_qos" ref="A1:E2" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:E2" xr:uid="{99A6AB2F-E55E-504E-B11A-162B09601887}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{8EFB6D15-9626-CF4A-AD61-6B5246860000}" name="HOSTNAME"/>
+    <tableColumn id="2" xr3:uid="{846B05A6-96F9-534F-86C6-494DCDC8AF81}" name="NAME"/>
+    <tableColumn id="3" xr3:uid="{9CE04D44-D082-C645-B332-5B7B98E15E28}" name="MATCH"/>
+    <tableColumn id="4" xr3:uid="{D736C4C1-9ED2-DC4B-A3E1-CB7F4EE4A0CF}" name="MATCH_VALUE"/>
+    <tableColumn id="5" xr3:uid="{FFD1003C-ECD2-F84F-A234-693688246572}" name="STATUS"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{45475B56-5B0D-8C4B-8705-9CCA614A9FE8}" name="policy_map_qos" displayName="policy_map_qos" ref="A1:E2" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:E2" xr:uid="{45475B56-5B0D-8C4B-8705-9CCA614A9FE8}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{1B5F31C1-EEE8-CF40-90C3-386C257EFCE2}" name="HOSTNAME" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{442C2D97-234F-B042-946E-F9ADA04A73B7}" name="NAME"/>
+    <tableColumn id="3" xr3:uid="{5CB2C467-864E-5341-883D-4F1B2A7E60D9}" name="CLASS_MAP_NAME"/>
+    <tableColumn id="4" xr3:uid="{1578379F-20DA-DF4A-9024-11E6CBF3BBB6}" name="QOS_GROUP"/>
+    <tableColumn id="5" xr3:uid="{92ADDB5D-0375-2540-9A76-3F2790D3EFD6}" name="STATUS" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D160ABCF-CDD5-F24F-B6E2-CC10F6567D78}" name="nxos_features" displayName="nxos_features" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="95" headerRowBorderDxfId="94" tableBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D160ABCF-CDD5-F24F-B6E2-CC10F6567D78}" name="nxos_features" displayName="nxos_features" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="109" headerRowBorderDxfId="108" tableBorderDxfId="107">
   <autoFilter ref="A1:D2" xr:uid="{15558EBF-F85A-A54A-9CF1-6A04C78B7201}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8A2FA099-FDDE-0746-AE77-C7D431D3C178}" name="HOSTNAME"/>
-    <tableColumn id="2" xr3:uid="{087A5ABC-CC88-1343-9752-40ACB66DD53A}" name="DEVICE_OS" dataDxfId="92">
+    <tableColumn id="2" xr3:uid="{087A5ABC-CC88-1343-9752-40ACB66DD53A}" name="DEVICE_OS" dataDxfId="106">
       <calculatedColumnFormula>IF(ISBLANK(nxos_features[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(nxos_features[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{8877F4A4-A003-9449-8947-A98C70CE9643}" name="FEATURE"/>
@@ -3958,12 +4339,39 @@
 </table>
 </file>
 
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{32860802-A7E9-EE42-A0DB-B05339B67AAA}" name="policy_map_queuing" displayName="policy_map_queuing" ref="A1:F2" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:F2" xr:uid="{32860802-A7E9-EE42-A0DB-B05339B67AAA}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{405987EC-581A-9346-8CD4-1A4054D35053}" name="HOSTNAME" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{9042E5BE-8E54-6045-AA92-9D5286E49691}" name="NAME"/>
+    <tableColumn id="3" xr3:uid="{F4325C53-5339-554F-9715-7D0678F95371}" name="QUEUING"/>
+    <tableColumn id="4" xr3:uid="{4B911A76-6184-6F4A-A4BC-F1707EC965A8}" name="PRIORITY_LEVEL"/>
+    <tableColumn id="5" xr3:uid="{0117B804-0385-2B4F-BB3C-09B3561B4405}" name="BANDWIDTH"/>
+    <tableColumn id="6" xr3:uid="{CC791DB7-40C5-424D-8C6F-F371E73E60E7}" name="STATUS" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{FB407252-0508-C74E-B74D-49FEA84EEF97}" name="system_qos_queuing_output" displayName="system_qos_queuing_output" ref="A1:C2" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="A1:C2" xr:uid="{FB407252-0508-C74E-B74D-49FEA84EEF97}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{997CFA8A-2941-C34C-8F4B-784F1F9A2249}" name="HOSTNAME" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{62964594-9617-F845-BB6D-29A5BBDAB9B0}" name="NAME"/>
+    <tableColumn id="3" xr3:uid="{363CB8A1-32CA-D149-BCA9-D39E24A72C5F}" name="STATUS" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1C28111F-59C8-6349-8EC8-6897FC5F5C3A}" name="port_channels" displayName="port_channels" ref="A1:H2" insertRow="1" totalsRowShown="0" tableBorderDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1C28111F-59C8-6349-8EC8-6897FC5F5C3A}" name="port_channels" displayName="port_channels" ref="A1:H2" insertRow="1" totalsRowShown="0" tableBorderDxfId="105">
   <autoFilter ref="A1:H2" xr:uid="{CBC26200-4209-3849-9A7D-C5767C11C244}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7BAF873C-B8C3-E24E-AD51-5E071B2CEB26}" name="HOSTNAME"/>
-    <tableColumn id="2" xr3:uid="{259B4B4F-D29B-6F47-B76D-7BDDB5CFF220}" name="DEVICE_OS" dataDxfId="90">
+    <tableColumn id="2" xr3:uid="{259B4B4F-D29B-6F47-B76D-7BDDB5CFF220}" name="DEVICE_OS" dataDxfId="104">
       <calculatedColumnFormula>IF(ISBLANK(port_channels[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(port_channels[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{91FEB763-37C9-F54B-A3A9-5EE4EC230ED6}" name="INTERFACE"/>
@@ -3981,8 +4389,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DF33A378-F683-464D-B600-B63F32BDB3C9}" name="vrfs" displayName="vrfs" ref="A1:B2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{509D4756-A42E-114E-80F3-9D83D65AD5D8}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7FCF5EA8-1765-3940-8F7F-3D48D823D788}" name="NAME" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{942CE1F9-B9BF-F64E-8BF3-470081B77DDF}" name="RD" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{7FCF5EA8-1765-3940-8F7F-3D48D823D788}" name="NAME" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{942CE1F9-B9BF-F64E-8BF3-470081B77DDF}" name="RD" dataDxfId="102"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3993,11 +4401,11 @@
   <autoFilter ref="A1:H2" xr:uid="{A1F75A44-21CF-004B-8425-2DD34E03999C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{706BFCCC-5CCB-DA44-9DF3-112D9FC3BA05}" name="HOSTNAME"/>
-    <tableColumn id="3" xr3:uid="{1615B641-38A5-F84C-B425-C5C2B0A97AD5}" name="DEVICE_OS" dataDxfId="87">
+    <tableColumn id="3" xr3:uid="{1615B641-38A5-F84C-B425-C5C2B0A97AD5}" name="DEVICE_OS" dataDxfId="101">
       <calculatedColumnFormula>IF(ISBLANK(device_vrfs[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(device_vrfs[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{45F93218-1BB6-844A-9CA4-DD101878B936}" name="VRF"/>
-    <tableColumn id="7" xr3:uid="{AEF4F533-EA19-6749-9BBA-6A212F98D99A}" name="RD" dataDxfId="86">
+    <tableColumn id="7" xr3:uid="{AEF4F533-EA19-6749-9BBA-6A212F98D99A}" name="RD" dataDxfId="100">
       <calculatedColumnFormula>IF(ISBLANK(device_vrfs[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(device_vrfs[[#This Row],[VRF]],vrfs[NAME],vrfs[RD]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{21AD3C2D-D1E0-814C-BCBF-C1AEF70A40EE}" name="DESCRIPTION"/>
@@ -4014,13 +4422,13 @@
   <autoFilter ref="A1:G2" xr:uid="{C3970CA1-6E2C-C447-9BFB-1AB7967FF334}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E67AA695-2B32-D945-BD4F-1666452C64C8}" name="HOSTNAME"/>
-    <tableColumn id="4" xr3:uid="{FD19EBAC-CB04-0A40-BA8B-D0BE4CCBBA41}" name="DEVICE_OS" dataDxfId="85">
+    <tableColumn id="4" xr3:uid="{FD19EBAC-CB04-0A40-BA8B-D0BE4CCBBA41}" name="DEVICE_OS" dataDxfId="99">
       <calculatedColumnFormula>IF(ISBLANK(ospf[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(ospf[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{D3C42C66-3DA0-3748-88FC-46126DD845FF}" name="VRF"/>
     <tableColumn id="18" xr3:uid="{D649DB6A-A0F0-2A4B-AC4F-2445F55575AD}" name="OSPF_ID"/>
-    <tableColumn id="19" xr3:uid="{A6FA7A3A-EA03-7146-A1C7-2B2F831A7326}" name="OSPF_ROUTER_ID" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{EF667B63-5704-1541-A7A0-DAECF2E40AE8}" name="REFERENCE_BANDWIDTH" dataDxfId="83"/>
+    <tableColumn id="19" xr3:uid="{A6FA7A3A-EA03-7146-A1C7-2B2F831A7326}" name="OSPF_ROUTER_ID" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{EF667B63-5704-1541-A7A0-DAECF2E40AE8}" name="REFERENCE_BANDWIDTH" dataDxfId="97"/>
     <tableColumn id="9" xr3:uid="{22492105-FDAF-C54C-8187-669D12E64D0D}" name="STATUS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4033,13 +4441,13 @@
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{1745545E-5B6E-7345-A78B-D6204938F96E}" name="HOSTNAME"/>
     <tableColumn id="2" xr3:uid="{D3B63833-3EC7-7646-BE68-0F336F6461FC}" name="VRF"/>
-    <tableColumn id="7" xr3:uid="{249A88F6-760F-4F77-B377-DE8FEE13454F}" name="DEVICE_OS" dataDxfId="82">
+    <tableColumn id="7" xr3:uid="{249A88F6-760F-4F77-B377-DE8FEE13454F}" name="DEVICE_OS" dataDxfId="96">
       <calculatedColumnFormula>IF(ISBLANK(loopbacks[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(loopbacks[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{CF28568B-30CB-9A4C-84A0-65AD2F529CD9}" name="LO_ID"/>
-    <tableColumn id="4" xr3:uid="{80D1A26E-FA76-D74E-8315-DD3C64461A10}" name="IP_ADDRESS" dataDxfId="81"/>
-    <tableColumn id="14" xr3:uid="{363298CE-69B3-864C-9214-74A6B5AB7141}" name="ENABLE_OSPF" dataDxfId="80"/>
-    <tableColumn id="5" xr3:uid="{FBE12430-F154-7243-A2C6-4C583194D3F8}" name="OSPF_ID" dataDxfId="79">
+    <tableColumn id="4" xr3:uid="{80D1A26E-FA76-D74E-8315-DD3C64461A10}" name="IP_ADDRESS" dataDxfId="95"/>
+    <tableColumn id="14" xr3:uid="{363298CE-69B3-864C-9214-74A6B5AB7141}" name="ENABLE_OSPF" dataDxfId="94"/>
+    <tableColumn id="5" xr3:uid="{FBE12430-F154-7243-A2C6-4C583194D3F8}" name="OSPF_ID" dataDxfId="93">
       <calculatedColumnFormula array="1">IF(loopbacks[[#This Row],[ENABLE_OSPF]] = "No","",_xlfn.XLOOKUP(_xlfn.SINGLE(loopbacks[HOSTNAME])&amp;loopbacks[[#This Row],[VRF]],ospf[HOSTNAME]&amp;ospf[VRF],ospf[OSPF_ID]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{175A7AB2-1C5C-A549-B557-5E248E423806}" name="OSPF_AREA"/>
@@ -4057,10 +4465,10 @@
   <autoFilter ref="A1:W2" xr:uid="{DD216AC4-FD74-6E47-B4CC-3F9FC894EFFD}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{1FBD31D9-874E-AF4E-A3D1-141126E87D87}" name="HOSTNAME"/>
-    <tableColumn id="2" xr3:uid="{C3A2D69F-5FE5-D345-9794-E2ED301C4D34}" name="DEVICE_OS" dataDxfId="78">
+    <tableColumn id="2" xr3:uid="{C3A2D69F-5FE5-D345-9794-E2ED301C4D34}" name="DEVICE_OS" dataDxfId="92">
       <calculatedColumnFormula>IF(ISBLANK(interfaces[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(interfaces[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{B104D4FB-806E-EF4E-BC7A-5368F78F484C}" name="DEVICE_TYPE" dataDxfId="77">
+    <tableColumn id="24" xr3:uid="{B104D4FB-806E-EF4E-BC7A-5368F78F484C}" name="DEVICE_TYPE" dataDxfId="91">
       <calculatedColumnFormula>IF(ISBLANK(interfaces[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(interfaces[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_TYPE]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{C130E233-5749-9C41-8467-517B8E4098A0}" name="INTERFACE"/>
@@ -4068,7 +4476,7 @@
     <tableColumn id="5" xr3:uid="{62E47652-D42D-9247-A7EF-78ECEE9BD10E}" name="VRF"/>
     <tableColumn id="13" xr3:uid="{E2CE50A5-8FCC-5945-A33E-490E37B5B251}" name="IP_ADDRESS"/>
     <tableColumn id="6" xr3:uid="{D72F0F76-AFC8-5A40-A52D-7C082916411E}" name="ENABLE_OSPF"/>
-    <tableColumn id="7" xr3:uid="{F0FDD87C-D7F7-C94C-9554-C131A9109A26}" name="OSPF_ID" dataDxfId="76">
+    <tableColumn id="7" xr3:uid="{F0FDD87C-D7F7-C94C-9554-C131A9109A26}" name="OSPF_ID" dataDxfId="90">
       <calculatedColumnFormula array="1">IF(interfaces[[#This Row],[ENABLE_OSPF]] = "No","",_xlfn.XLOOKUP(_xlfn.SINGLE(interfaces[HOSTNAME])&amp;interfaces[[#This Row],[VRF]],ospf[HOSTNAME]&amp;ospf[VRF],ospf[OSPF_ID]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{249B22EF-515D-C242-810D-1ADBEF5DCACC}" name="OSPF_AREA"/>
@@ -4091,19 +4499,19 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{EF182424-B364-2E40-B9E7-2D19AD52806B}" name="as_path_access_list" displayName="as_path_access_list" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{EF182424-B364-2E40-B9E7-2D19AD52806B}" name="as_path_access_list" displayName="as_path_access_list" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="89" dataDxfId="87" headerRowBorderDxfId="88">
   <autoFilter ref="A1:H2" xr:uid="{46C7A6E1-AD48-0148-8EAE-A397341A8F27}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{95E55C61-E799-7E4C-87D2-32EB02EDF339}" name="HOSTNAME" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{0260098B-0476-9F49-96A3-CFF841B40E86}" name="DEVICE_OS" dataDxfId="71">
+    <tableColumn id="1" xr3:uid="{95E55C61-E799-7E4C-87D2-32EB02EDF339}" name="HOSTNAME" dataDxfId="86"/>
+    <tableColumn id="6" xr3:uid="{0260098B-0476-9F49-96A3-CFF841B40E86}" name="DEVICE_OS" dataDxfId="85">
       <calculatedColumnFormula>IF(ISBLANK(as_path_access_list[[#This Row],[HOSTNAME]]),"",_xlfn.XLOOKUP(as_path_access_list[[#This Row],[HOSTNAME]],devices[HOSTNAME],devices[DEVICE_OS]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8D31D796-4B4A-D547-9FBD-4199CC9BE96F}" name="NAME" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{76DD162F-BE3A-A446-8FFF-A1BBEE98D558}" name="LIST_NUMBER" dataDxfId="69"/>
-    <tableColumn id="9" xr3:uid="{C7FA814C-3D8C-4C46-A361-F3B427EF7CEC}" name="SEQUENCE" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{6D448DBA-7BE6-A24B-94B2-F8F9DC0D5202}" name="ACTION" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{D745686C-80DD-7B4B-B1EB-891B99684EE6}" name="REGULAR_EXPRESSION" dataDxfId="66"/>
-    <tableColumn id="7" xr3:uid="{86F6B4B2-27A7-C648-BBA6-A86FB7BA76CE}" name="STATUS" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{8D31D796-4B4A-D547-9FBD-4199CC9BE96F}" name="NAME" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{76DD162F-BE3A-A446-8FFF-A1BBEE98D558}" name="LIST_NUMBER" dataDxfId="83"/>
+    <tableColumn id="9" xr3:uid="{C7FA814C-3D8C-4C46-A361-F3B427EF7CEC}" name="SEQUENCE" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{6D448DBA-7BE6-A24B-94B2-F8F9DC0D5202}" name="ACTION" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{D745686C-80DD-7B4B-B1EB-891B99684EE6}" name="REGULAR_EXPRESSION" dataDxfId="80"/>
+    <tableColumn id="7" xr3:uid="{86F6B4B2-27A7-C648-BBA6-A86FB7BA76CE}" name="STATUS" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4416,7 +4824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A47D4A-1E9B-EF4E-8065-17402CAF3208}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView zoomScale="136" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="I8" sqref="I8:I9"/>
     </sheetView>
   </sheetViews>
@@ -5338,1592 +5746,128 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC7AA23-B9D3-1B4F-A22F-9C8BE49A719A}">
-  <dimension ref="A1:X151"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A749FA-065A-F14B-AEB9-76B7A5C28275}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" zoomScale="244" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+    <sheetView zoomScale="397" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" t="s">
-        <v>139</v>
-      </c>
-      <c r="J1" t="s">
-        <v>140</v>
-      </c>
-      <c r="K1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" t="s">
-        <v>141</v>
-      </c>
-      <c r="M1" t="s">
-        <v>142</v>
-      </c>
-      <c r="N1" t="s">
-        <v>143</v>
-      </c>
-      <c r="O1" t="s">
-        <v>144</v>
-      </c>
-      <c r="P1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>146</v>
-      </c>
-      <c r="R1" t="s">
-        <v>147</v>
-      </c>
-      <c r="S1" t="s">
-        <v>123</v>
-      </c>
-      <c r="T1" t="s">
-        <v>124</v>
-      </c>
-      <c r="U1" t="s">
-        <v>148</v>
-      </c>
-      <c r="V1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="W1" t="s">
-        <v>149</v>
-      </c>
-      <c r="X1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>154</v>
-      </c>
-      <c r="J2" t="s">
-        <v>155</v>
-      </c>
-      <c r="K2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" t="s">
-        <v>156</v>
-      </c>
-      <c r="M2" t="s">
-        <v>98</v>
-      </c>
-      <c r="N2" cm="1">
-        <f t="array" ref="N2">_xlfn.UNIQUE(prefix_list[NAME])</f>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{A3F5CD57-7397-BF47-9FDC-2A3082BA3707}">
+      <formula1>"dscp"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{D98AD805-86CE-E24C-B911-C5F735E04331}">
+      <formula1>"present,absent,ignored"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{114D7D5A-8695-554C-8926-03C0B1E98EBA}">
+          <x14:formula1>
+            <xm:f>devices!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F49DFA-A361-B342-B3F4-63137E2B5FF6}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView zoomScale="400" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="O2" cm="1">
-        <f t="array" ref="O2">_xlfn.UNIQUE(as_path_access_list[[#This Row],[NAME]])</f>
-        <v>0</v>
-      </c>
-      <c r="P2" cm="1">
-        <f t="array" ref="P2">_xlfn.UNIQUE(route_map[NAME])</f>
-        <v>0</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>157</v>
-      </c>
-      <c r="R2" t="s">
-        <v>118</v>
-      </c>
-      <c r="S2" cm="1">
-        <f t="array" ref="S2">_xlfn.UNIQUE(bgp_peer_session[UPDATE_SOURCE_LOOPBACK])</f>
-        <v>0</v>
-      </c>
-      <c r="T2" cm="1">
-        <f t="array" ref="T2">_xlfn.UNIQUE(bgp_peer_policy[NAME])</f>
-        <v>0</v>
-      </c>
-      <c r="U2" t="s">
-        <v>158</v>
-      </c>
-      <c r="V2" t="s">
-        <v>17</v>
-      </c>
-      <c r="W2" t="s">
-        <v>25</v>
-      </c>
-      <c r="X2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>164</v>
-      </c>
-      <c r="K3" t="s">
-        <v>165</v>
-      </c>
-      <c r="L3" t="s">
-        <v>166</v>
-      </c>
-      <c r="M3" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>167</v>
-      </c>
-      <c r="U3" t="s">
-        <v>168</v>
-      </c>
-      <c r="V3" t="s">
-        <v>169</v>
-      </c>
-      <c r="W3" t="s">
-        <v>20</v>
-      </c>
-      <c r="X3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>174</v>
-      </c>
-      <c r="K4" t="s">
-        <v>175</v>
-      </c>
-      <c r="V4" t="s">
-        <v>18</v>
-      </c>
-      <c r="W4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D5" t="s">
-        <v>178</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>179</v>
-      </c>
-      <c r="W5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>180</v>
-      </c>
-      <c r="C6" t="s">
-        <v>181</v>
-      </c>
-      <c r="D6" t="s">
-        <v>182</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="J6" t="s">
-        <v>183</v>
-      </c>
-      <c r="W6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D7" t="s">
-        <v>186</v>
-      </c>
-      <c r="E7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="J7" t="s">
-        <v>187</v>
-      </c>
-      <c r="W7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C8" t="s">
-        <v>189</v>
-      </c>
-      <c r="D8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
-      <c r="J8" t="s">
-        <v>191</v>
-      </c>
-      <c r="W8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>192</v>
-      </c>
-      <c r="C9" t="s">
-        <v>193</v>
-      </c>
-      <c r="D9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="J9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>196</v>
-      </c>
-      <c r="C10" t="s">
-        <v>197</v>
-      </c>
-      <c r="D10" t="s">
-        <v>198</v>
-      </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10">
-        <v>9</v>
-      </c>
-      <c r="J10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>200</v>
-      </c>
-      <c r="C11" t="s">
-        <v>201</v>
-      </c>
-      <c r="D11" t="s">
-        <v>202</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>204</v>
-      </c>
-      <c r="C12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D12" t="s">
-        <v>206</v>
-      </c>
-      <c r="E12" t="s">
-        <v>207</v>
-      </c>
-      <c r="H12">
-        <v>11</v>
-      </c>
-      <c r="J12" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>209</v>
-      </c>
-      <c r="C13" t="s">
-        <v>210</v>
-      </c>
-      <c r="D13" t="s">
-        <v>211</v>
-      </c>
-      <c r="E13" t="s">
-        <v>212</v>
-      </c>
-      <c r="H13">
-        <v>12</v>
-      </c>
-      <c r="J13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>214</v>
-      </c>
-      <c r="C14" t="s">
-        <v>215</v>
-      </c>
-      <c r="E14" t="s">
-        <v>216</v>
-      </c>
-      <c r="H14">
-        <v>13</v>
-      </c>
-      <c r="J14" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>218</v>
-      </c>
-      <c r="C15" t="s">
-        <v>219</v>
-      </c>
-      <c r="E15" t="s">
-        <v>220</v>
-      </c>
-      <c r="H15">
+      <c r="B1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J15" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>222</v>
-      </c>
-      <c r="C16" t="s">
-        <v>223</v>
-      </c>
-      <c r="E16" t="s">
-        <v>224</v>
-      </c>
-      <c r="H16">
-        <v>15</v>
-      </c>
-      <c r="J16" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>226</v>
-      </c>
-      <c r="C17" t="s">
-        <v>227</v>
-      </c>
-      <c r="E17" t="s">
-        <v>228</v>
-      </c>
-      <c r="H17">
-        <v>16</v>
-      </c>
-      <c r="J17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>230</v>
-      </c>
-      <c r="C18" t="s">
-        <v>231</v>
-      </c>
-      <c r="E18" t="s">
-        <v>232</v>
-      </c>
-      <c r="H18">
-        <v>17</v>
-      </c>
-      <c r="J18" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>234</v>
-      </c>
-      <c r="C19" t="s">
-        <v>235</v>
-      </c>
-      <c r="E19" t="s">
-        <v>236</v>
-      </c>
-      <c r="H19">
-        <v>18</v>
-      </c>
-      <c r="J19" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>238</v>
-      </c>
-      <c r="C20" t="s">
-        <v>239</v>
-      </c>
-      <c r="E20" t="s">
-        <v>240</v>
-      </c>
-      <c r="H20">
-        <v>19</v>
-      </c>
-      <c r="J20" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>242</v>
-      </c>
-      <c r="E21" t="s">
-        <v>243</v>
-      </c>
-      <c r="H21">
-        <v>20</v>
-      </c>
-      <c r="J21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>245</v>
-      </c>
-      <c r="E22" t="s">
-        <v>246</v>
-      </c>
-      <c r="H22">
-        <v>21</v>
-      </c>
-      <c r="J22" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>248</v>
-      </c>
-      <c r="E23" t="s">
-        <v>249</v>
-      </c>
-      <c r="H23">
-        <v>22</v>
-      </c>
-      <c r="J23" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>251</v>
-      </c>
-      <c r="E24" t="s">
-        <v>252</v>
-      </c>
-      <c r="H24">
-        <v>23</v>
-      </c>
-      <c r="J24" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>254</v>
-      </c>
-      <c r="E25" t="s">
-        <v>255</v>
-      </c>
-      <c r="H25">
-        <v>24</v>
-      </c>
-      <c r="J25" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>257</v>
-      </c>
-      <c r="E26" t="s">
-        <v>258</v>
-      </c>
-      <c r="H26">
-        <v>25</v>
-      </c>
-      <c r="J26" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>260</v>
-      </c>
-      <c r="E27" t="s">
-        <v>261</v>
-      </c>
-      <c r="H27">
-        <v>26</v>
-      </c>
-      <c r="J27" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
-        <v>263</v>
-      </c>
-      <c r="E28" t="s">
-        <v>264</v>
-      </c>
-      <c r="H28">
-        <v>27</v>
-      </c>
-      <c r="J28" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>266</v>
-      </c>
-      <c r="E29" t="s">
-        <v>267</v>
-      </c>
-      <c r="H29">
-        <v>28</v>
-      </c>
-      <c r="J29" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>269</v>
-      </c>
-      <c r="E30" t="s">
-        <v>270</v>
-      </c>
-      <c r="H30">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>271</v>
-      </c>
-      <c r="E31" t="s">
-        <v>272</v>
-      </c>
-      <c r="H31">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>273</v>
-      </c>
-      <c r="E32" t="s">
-        <v>274</v>
-      </c>
-      <c r="H32">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
-        <v>275</v>
-      </c>
-      <c r="E33" t="s">
-        <v>276</v>
-      </c>
-      <c r="H33">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>277</v>
-      </c>
-      <c r="E34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>278</v>
-      </c>
-      <c r="E35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
-        <v>279</v>
-      </c>
-      <c r="E36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
-        <v>280</v>
-      </c>
-      <c r="E37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
-        <v>281</v>
-      </c>
-      <c r="E38" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
-        <v>283</v>
-      </c>
-      <c r="E39" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
-        <v>285</v>
-      </c>
-      <c r="E40" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
-        <v>287</v>
-      </c>
-      <c r="E41" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C42" t="s">
-        <v>289</v>
-      </c>
-      <c r="E42" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
-        <v>291</v>
-      </c>
-      <c r="E43" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
-        <v>293</v>
-      </c>
-      <c r="E44" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C45" t="s">
-        <v>295</v>
-      </c>
-      <c r="E45" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C46" t="s">
-        <v>297</v>
-      </c>
-      <c r="E46" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C47" t="s">
-        <v>299</v>
-      </c>
-      <c r="E47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C48" t="s">
-        <v>300</v>
-      </c>
-      <c r="E48" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
-        <v>301</v>
-      </c>
-      <c r="E49" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C50" t="s">
-        <v>302</v>
-      </c>
-      <c r="E50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C51" t="s">
-        <v>303</v>
-      </c>
-      <c r="E51" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C52" t="s">
-        <v>304</v>
-      </c>
-      <c r="E52" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C53" t="s">
-        <v>305</v>
-      </c>
-      <c r="E53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C54" t="s">
-        <v>306</v>
-      </c>
-      <c r="E54" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C55" t="s">
-        <v>307</v>
-      </c>
-      <c r="E55" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C56" t="s">
-        <v>308</v>
-      </c>
-      <c r="E56" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C57" t="s">
-        <v>310</v>
-      </c>
-      <c r="E57" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C58" t="s">
-        <v>312</v>
-      </c>
-      <c r="E58" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C59" t="s">
-        <v>313</v>
-      </c>
-      <c r="E59" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C60" t="s">
-        <v>314</v>
-      </c>
-      <c r="E60" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C61" t="s">
-        <v>316</v>
-      </c>
-      <c r="E61" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C62" t="s">
-        <v>318</v>
-      </c>
-      <c r="E62" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C63" t="s">
-        <v>320</v>
-      </c>
-      <c r="E63" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C64" t="s">
-        <v>322</v>
-      </c>
-      <c r="E64" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C65" t="s">
-        <v>324</v>
-      </c>
-      <c r="E65" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C66" t="s">
-        <v>326</v>
-      </c>
-      <c r="E66" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C67" t="s">
-        <v>328</v>
-      </c>
-      <c r="E67" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C68" t="s">
-        <v>330</v>
-      </c>
-      <c r="E68" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C69" t="s">
-        <v>332</v>
-      </c>
-      <c r="E69" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C70" t="s">
-        <v>334</v>
-      </c>
-      <c r="E70" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C71" t="s">
-        <v>336</v>
-      </c>
-      <c r="E71" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C72" t="s">
-        <v>338</v>
-      </c>
-      <c r="E72" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C73" t="s">
-        <v>340</v>
-      </c>
-      <c r="E73" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C74" t="s">
-        <v>342</v>
-      </c>
-      <c r="E74" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C75" t="s">
-        <v>344</v>
-      </c>
-      <c r="E75" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C76" t="s">
-        <v>346</v>
-      </c>
-      <c r="E76" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C77" t="s">
-        <v>347</v>
-      </c>
-      <c r="E77" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C78" t="s">
-        <v>348</v>
-      </c>
-      <c r="E78" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C79" t="s">
-        <v>350</v>
-      </c>
-      <c r="E79" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C80" t="s">
-        <v>351</v>
-      </c>
-      <c r="E80" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C81" t="s">
-        <v>353</v>
-      </c>
-      <c r="E81" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C82" t="s">
-        <v>355</v>
-      </c>
-      <c r="E82" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C83" t="s">
-        <v>357</v>
-      </c>
-      <c r="E83" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C84" t="s">
-        <v>359</v>
-      </c>
-      <c r="E84" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C85" t="s">
-        <v>361</v>
-      </c>
-      <c r="E85" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C86" t="s">
-        <v>363</v>
-      </c>
-      <c r="E86" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C87" t="s">
-        <v>365</v>
-      </c>
-      <c r="E87" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="88" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C88" t="s">
-        <v>367</v>
-      </c>
-      <c r="E88" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="89" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C89" t="s">
-        <v>369</v>
-      </c>
-      <c r="E89" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="90" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C90" t="s">
-        <v>371</v>
-      </c>
-      <c r="E90" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="91" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C91" t="s">
-        <v>373</v>
-      </c>
-      <c r="E91" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="92" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C92" t="s">
-        <v>375</v>
-      </c>
-      <c r="E92" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="93" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C93" t="s">
-        <v>377</v>
-      </c>
-      <c r="E93" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="94" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C94" t="s">
-        <v>379</v>
-      </c>
-      <c r="E94" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="95" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C95" t="s">
-        <v>381</v>
-      </c>
-      <c r="E95" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="96" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C96" t="s">
-        <v>383</v>
-      </c>
-      <c r="E96" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C97" t="s">
-        <v>385</v>
-      </c>
-      <c r="E97" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C98" t="s">
-        <v>387</v>
-      </c>
-      <c r="E98" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C99" t="s">
-        <v>389</v>
-      </c>
-      <c r="E99" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C100" t="s">
-        <v>391</v>
-      </c>
-      <c r="E100" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C101" t="s">
-        <v>393</v>
-      </c>
-      <c r="E101" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C102" t="s">
-        <v>395</v>
-      </c>
-      <c r="E102" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C103" t="s">
-        <v>397</v>
-      </c>
-      <c r="E103" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C104" t="s">
-        <v>399</v>
-      </c>
-      <c r="E104" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="105" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C105" t="s">
-        <v>401</v>
-      </c>
-      <c r="E105" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="106" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C106" t="s">
-        <v>403</v>
-      </c>
-      <c r="E106" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="107" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C107" t="s">
-        <v>405</v>
-      </c>
-      <c r="E107" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="108" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C108" t="s">
-        <v>407</v>
-      </c>
-      <c r="E108" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="109" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C109" t="s">
-        <v>408</v>
-      </c>
-      <c r="E109" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="110" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C110" t="s">
-        <v>409</v>
-      </c>
-      <c r="E110" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="111" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C111" t="s">
-        <v>410</v>
-      </c>
-      <c r="E111" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="112" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C112" t="s">
-        <v>411</v>
-      </c>
-      <c r="E112" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C113" t="s">
-        <v>413</v>
-      </c>
-      <c r="E113" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C114" t="s">
-        <v>415</v>
-      </c>
-      <c r="E114" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C115" t="s">
-        <v>416</v>
-      </c>
-      <c r="E115" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C116" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C117" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C118" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="119" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C119" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C120" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="121" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C121" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="122" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C122" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="123" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C123" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="124" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C124" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="125" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C125" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="126" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C126" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="127" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C127" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="128" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C128" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C129" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C130" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C131" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C132" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C133" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C134" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C135" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C136" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C137" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C138" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C139" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C140" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C141" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C142" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C143" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C144" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C145" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C146" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C147" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C148" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C149" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C150" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C151" t="s">
-        <v>447</v>
-      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="18"/>
+      <c r="E2" s="16"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{2AD40F9C-0C7C-5843-B1AE-8607B647E3E4}">
+      <formula1>"0,1,2,3,4,5,6,7"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{B39EDB3F-AFDB-1D46-A57C-E1746924E5A2}">
+      <formula1>"present,absent,ignored"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7741F14F-C829-5444-A4E0-27D9F1A0B8C7}">
+          <x14:formula1>
+            <xm:f>devices!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33184911-892D-2644-A4B7-C3B9EA5BF5DD}">
+          <x14:formula1>
+            <xm:f>'class_map_qos'!$B:$B</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6988,6 +5932,1719 @@
       </x14:dataValidations>
     </ext>
   </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A88D48-96FD-4449-9BD3-44406900C112}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="20"/>
+      <c r="F2" s="18"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{DF9B1528-0890-AC4E-9124-6DF5FF45C579}">
+      <formula1>"c-out-8q-q7,c-out-8q-q6,c-out-8q-q6,c-out-8q-q5,c-out-8q-q4,c-out-8q-q3,c-out-8q-q2,c-out-8q-q1,c-out-8q-q-default"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{48A6D76D-1606-A849-B2CD-3C37482AA77E}">
+      <formula1>"present,absent,ignored"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{62671338-CCAA-144A-A11C-3306B3739C15}">
+          <x14:formula1>
+            <xm:f>devices!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864792A1-4E8A-0F4E-B637-FEAE9B018102}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="20"/>
+      <c r="C2" s="18"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{EB6030D7-2FF9-BC43-824F-6DB49AE408C1}">
+      <formula1>"present,absent,ignored"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{4B5CAFEA-E4C5-3741-914A-50DDB76DE16A}">
+      <formula1>policy_map_queuing_name</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B7545F35-3EFD-E549-A051-87EE74633528}">
+          <x14:formula1>
+            <xm:f>devices!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC7AA23-B9D3-1B4F-A22F-9C8BE49A719A}">
+  <dimension ref="A1:X151"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="244" workbookViewId="0">
+      <selection activeCell="H116" sqref="H116"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M1" t="s">
+        <v>142</v>
+      </c>
+      <c r="N1" t="s">
+        <v>143</v>
+      </c>
+      <c r="O1" t="s">
+        <v>144</v>
+      </c>
+      <c r="P1" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>146</v>
+      </c>
+      <c r="R1" t="s">
+        <v>147</v>
+      </c>
+      <c r="S1" t="s">
+        <v>123</v>
+      </c>
+      <c r="T1" t="s">
+        <v>124</v>
+      </c>
+      <c r="U1" t="s">
+        <v>148</v>
+      </c>
+      <c r="V1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" t="s">
+        <v>149</v>
+      </c>
+      <c r="X1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" cm="1">
+        <f t="array" ref="N2">_xlfn.UNIQUE(prefix_list[NAME])</f>
+        <v>0</v>
+      </c>
+      <c r="O2" cm="1">
+        <f t="array" ref="O2">_xlfn.UNIQUE(as_path_access_list[[#This Row],[NAME]])</f>
+        <v>0</v>
+      </c>
+      <c r="P2" cm="1">
+        <f t="array" ref="P2">_xlfn.UNIQUE(route_map[NAME])</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>157</v>
+      </c>
+      <c r="R2" t="s">
+        <v>118</v>
+      </c>
+      <c r="S2" cm="1">
+        <f t="array" ref="S2">_xlfn.UNIQUE(bgp_peer_session[UPDATE_SOURCE_LOOPBACK])</f>
+        <v>0</v>
+      </c>
+      <c r="T2" cm="1">
+        <f t="array" ref="T2">_xlfn.UNIQUE(bgp_peer_policy[NAME])</f>
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>158</v>
+      </c>
+      <c r="V2" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L3" t="s">
+        <v>166</v>
+      </c>
+      <c r="M3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>167</v>
+      </c>
+      <c r="U3" t="s">
+        <v>168</v>
+      </c>
+      <c r="V3" t="s">
+        <v>169</v>
+      </c>
+      <c r="W3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>174</v>
+      </c>
+      <c r="K4" t="s">
+        <v>175</v>
+      </c>
+      <c r="V4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>179</v>
+      </c>
+      <c r="W5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>183</v>
+      </c>
+      <c r="W6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>187</v>
+      </c>
+      <c r="W7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>191</v>
+      </c>
+      <c r="W8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D11" t="s">
+        <v>202</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D12" t="s">
+        <v>206</v>
+      </c>
+      <c r="E12" t="s">
+        <v>207</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" t="s">
+        <v>212</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C14" t="s">
+        <v>215</v>
+      </c>
+      <c r="E14" t="s">
+        <v>216</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C15" t="s">
+        <v>219</v>
+      </c>
+      <c r="E15" t="s">
+        <v>220</v>
+      </c>
+      <c r="H15">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C16" t="s">
+        <v>223</v>
+      </c>
+      <c r="E16" t="s">
+        <v>224</v>
+      </c>
+      <c r="H16">
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" t="s">
+        <v>227</v>
+      </c>
+      <c r="E17" t="s">
+        <v>228</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C18" t="s">
+        <v>231</v>
+      </c>
+      <c r="E18" t="s">
+        <v>232</v>
+      </c>
+      <c r="H18">
+        <v>17</v>
+      </c>
+      <c r="J18" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" t="s">
+        <v>235</v>
+      </c>
+      <c r="E19" t="s">
+        <v>236</v>
+      </c>
+      <c r="H19">
+        <v>18</v>
+      </c>
+      <c r="J19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>238</v>
+      </c>
+      <c r="C20" t="s">
+        <v>239</v>
+      </c>
+      <c r="E20" t="s">
+        <v>240</v>
+      </c>
+      <c r="H20">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>242</v>
+      </c>
+      <c r="E21" t="s">
+        <v>243</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+      <c r="J21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>245</v>
+      </c>
+      <c r="E22" t="s">
+        <v>246</v>
+      </c>
+      <c r="H22">
+        <v>21</v>
+      </c>
+      <c r="J22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>248</v>
+      </c>
+      <c r="E23" t="s">
+        <v>249</v>
+      </c>
+      <c r="H23">
+        <v>22</v>
+      </c>
+      <c r="J23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>251</v>
+      </c>
+      <c r="E24" t="s">
+        <v>252</v>
+      </c>
+      <c r="H24">
+        <v>23</v>
+      </c>
+      <c r="J24" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>254</v>
+      </c>
+      <c r="E25" t="s">
+        <v>255</v>
+      </c>
+      <c r="H25">
+        <v>24</v>
+      </c>
+      <c r="J25" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>257</v>
+      </c>
+      <c r="E26" t="s">
+        <v>258</v>
+      </c>
+      <c r="H26">
+        <v>25</v>
+      </c>
+      <c r="J26" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>260</v>
+      </c>
+      <c r="E27" t="s">
+        <v>261</v>
+      </c>
+      <c r="H27">
+        <v>26</v>
+      </c>
+      <c r="J27" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>263</v>
+      </c>
+      <c r="E28" t="s">
+        <v>264</v>
+      </c>
+      <c r="H28">
+        <v>27</v>
+      </c>
+      <c r="J28" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>266</v>
+      </c>
+      <c r="E29" t="s">
+        <v>267</v>
+      </c>
+      <c r="H29">
+        <v>28</v>
+      </c>
+      <c r="J29" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>269</v>
+      </c>
+      <c r="E30" t="s">
+        <v>270</v>
+      </c>
+      <c r="H30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>271</v>
+      </c>
+      <c r="E31" t="s">
+        <v>272</v>
+      </c>
+      <c r="H31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>273</v>
+      </c>
+      <c r="E32" t="s">
+        <v>274</v>
+      </c>
+      <c r="H32">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>275</v>
+      </c>
+      <c r="E33" t="s">
+        <v>276</v>
+      </c>
+      <c r="H33">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>277</v>
+      </c>
+      <c r="E34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>278</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>279</v>
+      </c>
+      <c r="E36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>280</v>
+      </c>
+      <c r="E37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>281</v>
+      </c>
+      <c r="E38" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>283</v>
+      </c>
+      <c r="E39" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>285</v>
+      </c>
+      <c r="E40" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>287</v>
+      </c>
+      <c r="E41" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>289</v>
+      </c>
+      <c r="E42" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>291</v>
+      </c>
+      <c r="E43" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>293</v>
+      </c>
+      <c r="E44" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>295</v>
+      </c>
+      <c r="E45" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>297</v>
+      </c>
+      <c r="E46" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>299</v>
+      </c>
+      <c r="E47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>300</v>
+      </c>
+      <c r="E48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>301</v>
+      </c>
+      <c r="E49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>302</v>
+      </c>
+      <c r="E50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>303</v>
+      </c>
+      <c r="E51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>304</v>
+      </c>
+      <c r="E52" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>305</v>
+      </c>
+      <c r="E53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>306</v>
+      </c>
+      <c r="E54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>307</v>
+      </c>
+      <c r="E55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>308</v>
+      </c>
+      <c r="E56" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>310</v>
+      </c>
+      <c r="E57" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>312</v>
+      </c>
+      <c r="E58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
+        <v>313</v>
+      </c>
+      <c r="E59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>314</v>
+      </c>
+      <c r="E60" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>316</v>
+      </c>
+      <c r="E61" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
+        <v>318</v>
+      </c>
+      <c r="E62" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
+        <v>320</v>
+      </c>
+      <c r="E63" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>322</v>
+      </c>
+      <c r="E64" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>324</v>
+      </c>
+      <c r="E65" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>326</v>
+      </c>
+      <c r="E66" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>328</v>
+      </c>
+      <c r="E67" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>330</v>
+      </c>
+      <c r="E68" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>332</v>
+      </c>
+      <c r="E69" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>334</v>
+      </c>
+      <c r="E70" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>336</v>
+      </c>
+      <c r="E71" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>338</v>
+      </c>
+      <c r="E72" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>340</v>
+      </c>
+      <c r="E73" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>342</v>
+      </c>
+      <c r="E74" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>344</v>
+      </c>
+      <c r="E75" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>346</v>
+      </c>
+      <c r="E76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>347</v>
+      </c>
+      <c r="E77" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
+        <v>348</v>
+      </c>
+      <c r="E78" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="79" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
+        <v>350</v>
+      </c>
+      <c r="E79" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>351</v>
+      </c>
+      <c r="E80" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>353</v>
+      </c>
+      <c r="E81" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C82" t="s">
+        <v>355</v>
+      </c>
+      <c r="E82" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>357</v>
+      </c>
+      <c r="E83" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>359</v>
+      </c>
+      <c r="E84" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>361</v>
+      </c>
+      <c r="E85" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>363</v>
+      </c>
+      <c r="E86" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>365</v>
+      </c>
+      <c r="E87" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="88" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>367</v>
+      </c>
+      <c r="E88" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>369</v>
+      </c>
+      <c r="E89" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="90" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>371</v>
+      </c>
+      <c r="E90" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="91" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>373</v>
+      </c>
+      <c r="E91" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="92" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>375</v>
+      </c>
+      <c r="E92" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="93" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>377</v>
+      </c>
+      <c r="E93" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="94" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>379</v>
+      </c>
+      <c r="E94" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="95" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
+        <v>381</v>
+      </c>
+      <c r="E95" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="96" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
+        <v>383</v>
+      </c>
+      <c r="E96" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="97" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
+        <v>385</v>
+      </c>
+      <c r="E97" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="98" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
+        <v>387</v>
+      </c>
+      <c r="E98" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="99" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
+        <v>389</v>
+      </c>
+      <c r="E99" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="100" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C100" t="s">
+        <v>391</v>
+      </c>
+      <c r="E100" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="101" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C101" t="s">
+        <v>393</v>
+      </c>
+      <c r="E101" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="102" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C102" t="s">
+        <v>395</v>
+      </c>
+      <c r="E102" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="103" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C103" t="s">
+        <v>397</v>
+      </c>
+      <c r="E103" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="104" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C104" t="s">
+        <v>399</v>
+      </c>
+      <c r="E104" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="105" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C105" t="s">
+        <v>401</v>
+      </c>
+      <c r="E105" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="106" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C106" t="s">
+        <v>403</v>
+      </c>
+      <c r="E106" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="107" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C107" t="s">
+        <v>405</v>
+      </c>
+      <c r="E107" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="108" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C108" t="s">
+        <v>407</v>
+      </c>
+      <c r="E108" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="109" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C109" t="s">
+        <v>408</v>
+      </c>
+      <c r="E109" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="110" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C110" t="s">
+        <v>409</v>
+      </c>
+      <c r="E110" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="111" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C111" t="s">
+        <v>410</v>
+      </c>
+      <c r="E111" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="112" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C112" t="s">
+        <v>411</v>
+      </c>
+      <c r="E112" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C113" t="s">
+        <v>413</v>
+      </c>
+      <c r="E113" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C114" t="s">
+        <v>415</v>
+      </c>
+      <c r="E114" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="115" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C115" t="s">
+        <v>416</v>
+      </c>
+      <c r="E115" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C116" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C117" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="118" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C118" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="119" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C119" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="120" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C120" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="121" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C121" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="122" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C122" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="123" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C123" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="124" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C124" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="125" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C125" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="126" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C126" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="127" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C127" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="128" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C128" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C129" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C130" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C131" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C132" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C133" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C134" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C135" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C136" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C137" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C138" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C139" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C140" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C141" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C142" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C143" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C144" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C145" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C146" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C147" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C148" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C149" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C150" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C151" t="s">
+        <v>447</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>